<commit_message>
(SimpleProjects)Add Base Specifications & Delete gitkeep file
</commit_message>
<xml_diff>
--- a/SimpleProjects/Module/ParkingArea/1.Design/Image.xlsx
+++ b/SimpleProjects/Module/ParkingArea/1.Design/Image.xlsx
@@ -15,13 +15,13 @@
     <sheet name="Index" sheetId="2" r:id="rId1"/>
     <sheet name="History" sheetId="3" r:id="rId2"/>
     <sheet name="Functions" sheetId="1" r:id="rId3"/>
-    <sheet name="Project" sheetId="5" r:id="rId4"/>
+    <sheet name="Condition" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">Condition!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">Functions!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">History!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Index!#REF!</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="3">Project!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Write Date</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -95,11 +95,23 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>1) Parking Area</t>
+    <t>1) Kind of Car</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">2) </t>
+    <t>2) About Cost</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>FROM</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>TO</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>CONDITION</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -610,6 +622,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -741,21 +768,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5513,16 +5525,16 @@
       <c r="F1" s="9"/>
     </row>
     <row r="2" spans="2:48" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>
@@ -5631,400 +5643,400 @@
     </row>
     <row r="5" spans="2:48" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6"/>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
-      <c r="G5" s="57"/>
-      <c r="H5" s="57"/>
-      <c r="I5" s="57"/>
-      <c r="J5" s="57"/>
-      <c r="K5" s="57"/>
-      <c r="L5" s="57"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="57"/>
-      <c r="Q5" s="57"/>
-      <c r="R5" s="57"/>
-      <c r="S5" s="57"/>
-      <c r="T5" s="57"/>
-      <c r="U5" s="57"/>
-      <c r="V5" s="57"/>
-      <c r="W5" s="57"/>
-      <c r="X5" s="57"/>
-      <c r="Y5" s="57"/>
-      <c r="Z5" s="57"/>
-      <c r="AA5" s="57"/>
-      <c r="AB5" s="57"/>
-      <c r="AC5" s="57"/>
-      <c r="AD5" s="57"/>
-      <c r="AE5" s="57"/>
-      <c r="AF5" s="57"/>
-      <c r="AG5" s="57"/>
-      <c r="AH5" s="57"/>
-      <c r="AI5" s="57"/>
-      <c r="AJ5" s="57"/>
-      <c r="AK5" s="57"/>
-      <c r="AL5" s="57"/>
-      <c r="AM5" s="57"/>
-      <c r="AN5" s="57"/>
-      <c r="AO5" s="57"/>
-      <c r="AP5" s="57"/>
-      <c r="AQ5" s="57"/>
-      <c r="AR5" s="57"/>
-      <c r="AS5" s="57"/>
-      <c r="AT5" s="57"/>
-      <c r="AU5" s="57"/>
-      <c r="AV5" s="57"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="62"/>
+      <c r="F5" s="62"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="62"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="62"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="62"/>
+      <c r="P5" s="62"/>
+      <c r="Q5" s="62"/>
+      <c r="R5" s="62"/>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
+      <c r="V5" s="62"/>
+      <c r="W5" s="62"/>
+      <c r="X5" s="62"/>
+      <c r="Y5" s="62"/>
+      <c r="Z5" s="62"/>
+      <c r="AA5" s="62"/>
+      <c r="AB5" s="62"/>
+      <c r="AC5" s="62"/>
+      <c r="AD5" s="62"/>
+      <c r="AE5" s="62"/>
+      <c r="AF5" s="62"/>
+      <c r="AG5" s="62"/>
+      <c r="AH5" s="62"/>
+      <c r="AI5" s="62"/>
+      <c r="AJ5" s="62"/>
+      <c r="AK5" s="62"/>
+      <c r="AL5" s="62"/>
+      <c r="AM5" s="62"/>
+      <c r="AN5" s="62"/>
+      <c r="AO5" s="62"/>
+      <c r="AP5" s="62"/>
+      <c r="AQ5" s="62"/>
+      <c r="AR5" s="62"/>
+      <c r="AS5" s="62"/>
+      <c r="AT5" s="62"/>
+      <c r="AU5" s="62"/>
+      <c r="AV5" s="62"/>
     </row>
     <row r="6" spans="2:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="22"/>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58"/>
-      <c r="J6" s="58"/>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="58"/>
-      <c r="O6" s="58"/>
-      <c r="P6" s="58"/>
-      <c r="Q6" s="58"/>
-      <c r="R6" s="58"/>
-      <c r="S6" s="58"/>
-      <c r="T6" s="58"/>
-      <c r="U6" s="58"/>
-      <c r="V6" s="58"/>
-      <c r="W6" s="58"/>
-      <c r="X6" s="58"/>
-      <c r="Y6" s="58"/>
-      <c r="Z6" s="58"/>
-      <c r="AA6" s="58"/>
-      <c r="AB6" s="58"/>
-      <c r="AC6" s="58"/>
-      <c r="AD6" s="58"/>
-      <c r="AE6" s="58"/>
-      <c r="AF6" s="58"/>
-      <c r="AG6" s="58"/>
-      <c r="AH6" s="58"/>
-      <c r="AI6" s="58"/>
-      <c r="AJ6" s="58"/>
-      <c r="AK6" s="58"/>
-      <c r="AL6" s="58"/>
-      <c r="AM6" s="58"/>
-      <c r="AN6" s="58"/>
-      <c r="AO6" s="58"/>
-      <c r="AP6" s="58"/>
-      <c r="AQ6" s="58"/>
-      <c r="AR6" s="58"/>
-      <c r="AS6" s="58"/>
-      <c r="AT6" s="58"/>
-      <c r="AU6" s="58"/>
-      <c r="AV6" s="58"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="63"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="63"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="63"/>
+      <c r="T6" s="63"/>
+      <c r="U6" s="63"/>
+      <c r="V6" s="63"/>
+      <c r="W6" s="63"/>
+      <c r="X6" s="63"/>
+      <c r="Y6" s="63"/>
+      <c r="Z6" s="63"/>
+      <c r="AA6" s="63"/>
+      <c r="AB6" s="63"/>
+      <c r="AC6" s="63"/>
+      <c r="AD6" s="63"/>
+      <c r="AE6" s="63"/>
+      <c r="AF6" s="63"/>
+      <c r="AG6" s="63"/>
+      <c r="AH6" s="63"/>
+      <c r="AI6" s="63"/>
+      <c r="AJ6" s="63"/>
+      <c r="AK6" s="63"/>
+      <c r="AL6" s="63"/>
+      <c r="AM6" s="63"/>
+      <c r="AN6" s="63"/>
+      <c r="AO6" s="63"/>
+      <c r="AP6" s="63"/>
+      <c r="AQ6" s="63"/>
+      <c r="AR6" s="63"/>
+      <c r="AS6" s="63"/>
+      <c r="AT6" s="63"/>
+      <c r="AU6" s="63"/>
+      <c r="AV6" s="63"/>
     </row>
     <row r="7" spans="2:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="58"/>
-      <c r="D7" s="58"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="58"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
-      <c r="R7" s="58"/>
-      <c r="S7" s="58"/>
-      <c r="T7" s="58"/>
-      <c r="U7" s="58"/>
-      <c r="V7" s="58"/>
-      <c r="W7" s="58"/>
-      <c r="X7" s="58"/>
-      <c r="Y7" s="58"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="58"/>
-      <c r="AB7" s="58"/>
-      <c r="AC7" s="58"/>
-      <c r="AD7" s="58"/>
-      <c r="AE7" s="58"/>
-      <c r="AF7" s="58"/>
-      <c r="AG7" s="58"/>
-      <c r="AH7" s="58"/>
-      <c r="AI7" s="58"/>
-      <c r="AJ7" s="58"/>
-      <c r="AK7" s="58"/>
-      <c r="AL7" s="58"/>
-      <c r="AM7" s="58"/>
-      <c r="AN7" s="58"/>
-      <c r="AO7" s="58"/>
-      <c r="AP7" s="58"/>
-      <c r="AQ7" s="58"/>
-      <c r="AR7" s="58"/>
-      <c r="AS7" s="58"/>
-      <c r="AT7" s="58"/>
-      <c r="AU7" s="58"/>
-      <c r="AV7" s="58"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="63"/>
+      <c r="K7" s="63"/>
+      <c r="L7" s="63"/>
+      <c r="M7" s="63"/>
+      <c r="N7" s="63"/>
+      <c r="O7" s="63"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="63"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="63"/>
+      <c r="T7" s="63"/>
+      <c r="U7" s="63"/>
+      <c r="V7" s="63"/>
+      <c r="W7" s="63"/>
+      <c r="X7" s="63"/>
+      <c r="Y7" s="63"/>
+      <c r="Z7" s="63"/>
+      <c r="AA7" s="63"/>
+      <c r="AB7" s="63"/>
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="63"/>
+      <c r="AE7" s="63"/>
+      <c r="AF7" s="63"/>
+      <c r="AG7" s="63"/>
+      <c r="AH7" s="63"/>
+      <c r="AI7" s="63"/>
+      <c r="AJ7" s="63"/>
+      <c r="AK7" s="63"/>
+      <c r="AL7" s="63"/>
+      <c r="AM7" s="63"/>
+      <c r="AN7" s="63"/>
+      <c r="AO7" s="63"/>
+      <c r="AP7" s="63"/>
+      <c r="AQ7" s="63"/>
+      <c r="AR7" s="63"/>
+      <c r="AS7" s="63"/>
+      <c r="AT7" s="63"/>
+      <c r="AU7" s="63"/>
+      <c r="AV7" s="63"/>
     </row>
     <row r="8" spans="2:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
-      <c r="L8" s="58"/>
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
-      <c r="R8" s="58"/>
-      <c r="S8" s="58"/>
-      <c r="T8" s="58"/>
-      <c r="U8" s="58"/>
-      <c r="V8" s="58"/>
-      <c r="W8" s="58"/>
-      <c r="X8" s="58"/>
-      <c r="Y8" s="58"/>
-      <c r="Z8" s="58"/>
-      <c r="AA8" s="58"/>
-      <c r="AB8" s="58"/>
-      <c r="AC8" s="58"/>
-      <c r="AD8" s="58"/>
-      <c r="AE8" s="58"/>
-      <c r="AF8" s="58"/>
-      <c r="AG8" s="58"/>
-      <c r="AH8" s="58"/>
-      <c r="AI8" s="58"/>
-      <c r="AJ8" s="58"/>
-      <c r="AK8" s="58"/>
-      <c r="AL8" s="58"/>
-      <c r="AM8" s="58"/>
-      <c r="AN8" s="58"/>
-      <c r="AO8" s="58"/>
-      <c r="AP8" s="58"/>
-      <c r="AQ8" s="58"/>
-      <c r="AR8" s="58"/>
-      <c r="AS8" s="58"/>
-      <c r="AT8" s="58"/>
-      <c r="AU8" s="58"/>
-      <c r="AV8" s="58"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="63"/>
+      <c r="N8" s="63"/>
+      <c r="O8" s="63"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="63"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="63"/>
+      <c r="T8" s="63"/>
+      <c r="U8" s="63"/>
+      <c r="V8" s="63"/>
+      <c r="W8" s="63"/>
+      <c r="X8" s="63"/>
+      <c r="Y8" s="63"/>
+      <c r="Z8" s="63"/>
+      <c r="AA8" s="63"/>
+      <c r="AB8" s="63"/>
+      <c r="AC8" s="63"/>
+      <c r="AD8" s="63"/>
+      <c r="AE8" s="63"/>
+      <c r="AF8" s="63"/>
+      <c r="AG8" s="63"/>
+      <c r="AH8" s="63"/>
+      <c r="AI8" s="63"/>
+      <c r="AJ8" s="63"/>
+      <c r="AK8" s="63"/>
+      <c r="AL8" s="63"/>
+      <c r="AM8" s="63"/>
+      <c r="AN8" s="63"/>
+      <c r="AO8" s="63"/>
+      <c r="AP8" s="63"/>
+      <c r="AQ8" s="63"/>
+      <c r="AR8" s="63"/>
+      <c r="AS8" s="63"/>
+      <c r="AT8" s="63"/>
+      <c r="AU8" s="63"/>
+      <c r="AV8" s="63"/>
     </row>
     <row r="9" spans="2:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="11"/>
-      <c r="C9" s="59"/>
-      <c r="D9" s="59"/>
-      <c r="E9" s="59"/>
-      <c r="F9" s="59"/>
-      <c r="G9" s="59"/>
-      <c r="H9" s="59"/>
-      <c r="I9" s="59"/>
-      <c r="J9" s="59"/>
-      <c r="K9" s="59"/>
-      <c r="L9" s="59"/>
-      <c r="M9" s="59"/>
-      <c r="N9" s="59"/>
-      <c r="O9" s="59"/>
-      <c r="P9" s="59"/>
-      <c r="Q9" s="59"/>
-      <c r="R9" s="59"/>
-      <c r="S9" s="59"/>
-      <c r="T9" s="59"/>
-      <c r="U9" s="59"/>
-      <c r="V9" s="59"/>
-      <c r="W9" s="59"/>
-      <c r="X9" s="59"/>
-      <c r="Y9" s="59"/>
-      <c r="Z9" s="58"/>
-      <c r="AA9" s="58"/>
-      <c r="AB9" s="59"/>
-      <c r="AC9" s="59"/>
-      <c r="AD9" s="59"/>
-      <c r="AE9" s="59"/>
-      <c r="AF9" s="59"/>
-      <c r="AG9" s="59"/>
-      <c r="AH9" s="59"/>
-      <c r="AI9" s="59"/>
-      <c r="AJ9" s="59"/>
-      <c r="AK9" s="59"/>
-      <c r="AL9" s="59"/>
-      <c r="AM9" s="59"/>
-      <c r="AN9" s="59"/>
-      <c r="AO9" s="59"/>
-      <c r="AP9" s="59"/>
-      <c r="AQ9" s="59"/>
-      <c r="AR9" s="59"/>
-      <c r="AS9" s="59"/>
-      <c r="AT9" s="59"/>
-      <c r="AU9" s="59"/>
-      <c r="AV9" s="59"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="64"/>
+      <c r="K9" s="64"/>
+      <c r="L9" s="64"/>
+      <c r="M9" s="64"/>
+      <c r="N9" s="64"/>
+      <c r="O9" s="64"/>
+      <c r="P9" s="64"/>
+      <c r="Q9" s="64"/>
+      <c r="R9" s="64"/>
+      <c r="S9" s="64"/>
+      <c r="T9" s="64"/>
+      <c r="U9" s="64"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="64"/>
+      <c r="X9" s="64"/>
+      <c r="Y9" s="64"/>
+      <c r="Z9" s="63"/>
+      <c r="AA9" s="63"/>
+      <c r="AB9" s="64"/>
+      <c r="AC9" s="64"/>
+      <c r="AD9" s="64"/>
+      <c r="AE9" s="64"/>
+      <c r="AF9" s="64"/>
+      <c r="AG9" s="64"/>
+      <c r="AH9" s="64"/>
+      <c r="AI9" s="64"/>
+      <c r="AJ9" s="64"/>
+      <c r="AK9" s="64"/>
+      <c r="AL9" s="64"/>
+      <c r="AM9" s="64"/>
+      <c r="AN9" s="64"/>
+      <c r="AO9" s="64"/>
+      <c r="AP9" s="64"/>
+      <c r="AQ9" s="64"/>
+      <c r="AR9" s="64"/>
+      <c r="AS9" s="64"/>
+      <c r="AT9" s="64"/>
+      <c r="AU9" s="64"/>
+      <c r="AV9" s="64"/>
     </row>
     <row r="10" spans="2:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="11"/>
-      <c r="C10" s="60" t="s">
+      <c r="C10" s="65" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="60"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="60"/>
-      <c r="L10" s="60"/>
-      <c r="M10" s="60"/>
-      <c r="N10" s="60"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="60"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="60"/>
-      <c r="U10" s="60"/>
-      <c r="V10" s="60"/>
-      <c r="W10" s="60"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="60"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="65"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
+      <c r="U10" s="65"/>
+      <c r="V10" s="65"/>
+      <c r="W10" s="65"/>
+      <c r="X10" s="65"/>
+      <c r="Y10" s="65"/>
       <c r="Z10" s="29"/>
       <c r="AA10" s="14"/>
-      <c r="AB10" s="62" t="s">
+      <c r="AB10" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="AC10" s="62"/>
-      <c r="AD10" s="62"/>
-      <c r="AE10" s="62"/>
-      <c r="AF10" s="62"/>
-      <c r="AG10" s="62"/>
-      <c r="AH10" s="62"/>
-      <c r="AI10" s="62"/>
-      <c r="AJ10" s="62"/>
-      <c r="AK10" s="62"/>
-      <c r="AL10" s="62"/>
-      <c r="AM10" s="62"/>
-      <c r="AN10" s="62"/>
-      <c r="AO10" s="62"/>
-      <c r="AP10" s="62"/>
-      <c r="AQ10" s="62"/>
-      <c r="AR10" s="62"/>
-      <c r="AS10" s="62"/>
-      <c r="AT10" s="62"/>
-      <c r="AU10" s="62"/>
-      <c r="AV10" s="62"/>
+      <c r="AC10" s="67"/>
+      <c r="AD10" s="67"/>
+      <c r="AE10" s="67"/>
+      <c r="AF10" s="67"/>
+      <c r="AG10" s="67"/>
+      <c r="AH10" s="67"/>
+      <c r="AI10" s="67"/>
+      <c r="AJ10" s="67"/>
+      <c r="AK10" s="67"/>
+      <c r="AL10" s="67"/>
+      <c r="AM10" s="67"/>
+      <c r="AN10" s="67"/>
+      <c r="AO10" s="67"/>
+      <c r="AP10" s="67"/>
+      <c r="AQ10" s="67"/>
+      <c r="AR10" s="67"/>
+      <c r="AS10" s="67"/>
+      <c r="AT10" s="67"/>
+      <c r="AU10" s="67"/>
+      <c r="AV10" s="67"/>
     </row>
     <row r="11" spans="2:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="11"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="61"/>
-      <c r="N11" s="61"/>
-      <c r="O11" s="61"/>
-      <c r="P11" s="61"/>
-      <c r="Q11" s="61"/>
-      <c r="R11" s="61"/>
-      <c r="S11" s="61"/>
-      <c r="T11" s="61"/>
-      <c r="U11" s="61"/>
-      <c r="V11" s="61"/>
-      <c r="W11" s="61"/>
-      <c r="X11" s="61"/>
-      <c r="Y11" s="61"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
+      <c r="J11" s="66"/>
+      <c r="K11" s="66"/>
+      <c r="L11" s="66"/>
+      <c r="M11" s="66"/>
+      <c r="N11" s="66"/>
+      <c r="O11" s="66"/>
+      <c r="P11" s="66"/>
+      <c r="Q11" s="66"/>
+      <c r="R11" s="66"/>
+      <c r="S11" s="66"/>
+      <c r="T11" s="66"/>
+      <c r="U11" s="66"/>
+      <c r="V11" s="66"/>
+      <c r="W11" s="66"/>
+      <c r="X11" s="66"/>
+      <c r="Y11" s="66"/>
       <c r="Z11" s="29"/>
       <c r="AA11" s="30"/>
-      <c r="AB11" s="63"/>
-      <c r="AC11" s="63"/>
-      <c r="AD11" s="63"/>
-      <c r="AE11" s="63"/>
-      <c r="AF11" s="63"/>
-      <c r="AG11" s="63"/>
-      <c r="AH11" s="63"/>
-      <c r="AI11" s="63"/>
-      <c r="AJ11" s="63"/>
-      <c r="AK11" s="63"/>
-      <c r="AL11" s="63"/>
-      <c r="AM11" s="63"/>
-      <c r="AN11" s="63"/>
-      <c r="AO11" s="63"/>
-      <c r="AP11" s="63"/>
-      <c r="AQ11" s="63"/>
-      <c r="AR11" s="63"/>
-      <c r="AS11" s="63"/>
-      <c r="AT11" s="63"/>
-      <c r="AU11" s="63"/>
-      <c r="AV11" s="63"/>
+      <c r="AB11" s="68"/>
+      <c r="AC11" s="68"/>
+      <c r="AD11" s="68"/>
+      <c r="AE11" s="68"/>
+      <c r="AF11" s="68"/>
+      <c r="AG11" s="68"/>
+      <c r="AH11" s="68"/>
+      <c r="AI11" s="68"/>
+      <c r="AJ11" s="68"/>
+      <c r="AK11" s="68"/>
+      <c r="AL11" s="68"/>
+      <c r="AM11" s="68"/>
+      <c r="AN11" s="68"/>
+      <c r="AO11" s="68"/>
+      <c r="AP11" s="68"/>
+      <c r="AQ11" s="68"/>
+      <c r="AR11" s="68"/>
+      <c r="AS11" s="68"/>
+      <c r="AT11" s="68"/>
+      <c r="AU11" s="68"/>
+      <c r="AV11" s="68"/>
     </row>
     <row r="12" spans="2:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="61"/>
-      <c r="N12" s="61"/>
-      <c r="O12" s="61"/>
-      <c r="P12" s="61"/>
-      <c r="Q12" s="61"/>
-      <c r="R12" s="61"/>
-      <c r="S12" s="61"/>
-      <c r="T12" s="61"/>
-      <c r="U12" s="61"/>
-      <c r="V12" s="61"/>
-      <c r="W12" s="61"/>
-      <c r="X12" s="61"/>
-      <c r="Y12" s="61"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="66"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="66"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
+      <c r="O12" s="66"/>
+      <c r="P12" s="66"/>
+      <c r="Q12" s="66"/>
+      <c r="R12" s="66"/>
+      <c r="S12" s="66"/>
+      <c r="T12" s="66"/>
+      <c r="U12" s="66"/>
+      <c r="V12" s="66"/>
+      <c r="W12" s="66"/>
+      <c r="X12" s="66"/>
+      <c r="Y12" s="66"/>
       <c r="Z12" s="29"/>
       <c r="AA12" s="30"/>
-      <c r="AB12" s="63"/>
-      <c r="AC12" s="63"/>
-      <c r="AD12" s="63"/>
-      <c r="AE12" s="63"/>
-      <c r="AF12" s="63"/>
-      <c r="AG12" s="63"/>
-      <c r="AH12" s="63"/>
-      <c r="AI12" s="63"/>
-      <c r="AJ12" s="63"/>
-      <c r="AK12" s="63"/>
-      <c r="AL12" s="63"/>
-      <c r="AM12" s="63"/>
-      <c r="AN12" s="63"/>
-      <c r="AO12" s="63"/>
-      <c r="AP12" s="63"/>
-      <c r="AQ12" s="63"/>
-      <c r="AR12" s="63"/>
-      <c r="AS12" s="63"/>
-      <c r="AT12" s="63"/>
-      <c r="AU12" s="63"/>
-      <c r="AV12" s="63"/>
+      <c r="AB12" s="68"/>
+      <c r="AC12" s="68"/>
+      <c r="AD12" s="68"/>
+      <c r="AE12" s="68"/>
+      <c r="AF12" s="68"/>
+      <c r="AG12" s="68"/>
+      <c r="AH12" s="68"/>
+      <c r="AI12" s="68"/>
+      <c r="AJ12" s="68"/>
+      <c r="AK12" s="68"/>
+      <c r="AL12" s="68"/>
+      <c r="AM12" s="68"/>
+      <c r="AN12" s="68"/>
+      <c r="AO12" s="68"/>
+      <c r="AP12" s="68"/>
+      <c r="AQ12" s="68"/>
+      <c r="AR12" s="68"/>
+      <c r="AS12" s="68"/>
+      <c r="AT12" s="68"/>
+      <c r="AU12" s="68"/>
+      <c r="AV12" s="68"/>
     </row>
     <row r="13" spans="2:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="22"/>
@@ -6043,68 +6055,68 @@
       <c r="I14" s="22"/>
     </row>
     <row r="16" spans="2:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AK16" s="64" t="s">
+      <c r="AK16" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="AL16" s="64"/>
-      <c r="AM16" s="64"/>
-      <c r="AN16" s="64"/>
-      <c r="AO16" s="64"/>
-      <c r="AP16" s="64"/>
-      <c r="AQ16" s="64" t="s">
+      <c r="AL16" s="69"/>
+      <c r="AM16" s="69"/>
+      <c r="AN16" s="69"/>
+      <c r="AO16" s="69"/>
+      <c r="AP16" s="69"/>
+      <c r="AQ16" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="AR16" s="64"/>
-      <c r="AS16" s="64"/>
-      <c r="AT16" s="64"/>
-      <c r="AU16" s="64"/>
-      <c r="AV16" s="64"/>
+      <c r="AR16" s="69"/>
+      <c r="AS16" s="69"/>
+      <c r="AT16" s="69"/>
+      <c r="AU16" s="69"/>
+      <c r="AV16" s="69"/>
     </row>
     <row r="17" spans="37:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AK17" s="65"/>
-      <c r="AL17" s="65"/>
-      <c r="AM17" s="65"/>
-      <c r="AN17" s="65"/>
-      <c r="AO17" s="65"/>
-      <c r="AP17" s="65"/>
-      <c r="AQ17" s="65"/>
-      <c r="AR17" s="65"/>
-      <c r="AS17" s="65"/>
-      <c r="AT17" s="65"/>
-      <c r="AU17" s="65"/>
-      <c r="AV17" s="65"/>
+      <c r="AK17" s="70"/>
+      <c r="AL17" s="70"/>
+      <c r="AM17" s="70"/>
+      <c r="AN17" s="70"/>
+      <c r="AO17" s="70"/>
+      <c r="AP17" s="70"/>
+      <c r="AQ17" s="70"/>
+      <c r="AR17" s="70"/>
+      <c r="AS17" s="70"/>
+      <c r="AT17" s="70"/>
+      <c r="AU17" s="70"/>
+      <c r="AV17" s="70"/>
     </row>
     <row r="18" spans="37:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AK18" s="52">
+      <c r="AK18" s="57">
         <v>43955</v>
       </c>
-      <c r="AL18" s="52"/>
-      <c r="AM18" s="52"/>
-      <c r="AN18" s="52"/>
-      <c r="AO18" s="52"/>
-      <c r="AP18" s="52"/>
-      <c r="AQ18" s="54" t="s">
+      <c r="AL18" s="57"/>
+      <c r="AM18" s="57"/>
+      <c r="AN18" s="57"/>
+      <c r="AO18" s="57"/>
+      <c r="AP18" s="57"/>
+      <c r="AQ18" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="AR18" s="54"/>
-      <c r="AS18" s="54"/>
-      <c r="AT18" s="54"/>
-      <c r="AU18" s="54"/>
-      <c r="AV18" s="54"/>
+      <c r="AR18" s="59"/>
+      <c r="AS18" s="59"/>
+      <c r="AT18" s="59"/>
+      <c r="AU18" s="59"/>
+      <c r="AV18" s="59"/>
     </row>
     <row r="19" spans="37:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="AK19" s="53"/>
-      <c r="AL19" s="53"/>
-      <c r="AM19" s="53"/>
-      <c r="AN19" s="53"/>
-      <c r="AO19" s="53"/>
-      <c r="AP19" s="53"/>
-      <c r="AQ19" s="55"/>
-      <c r="AR19" s="55"/>
-      <c r="AS19" s="55"/>
-      <c r="AT19" s="55"/>
-      <c r="AU19" s="55"/>
-      <c r="AV19" s="55"/>
+      <c r="AK19" s="58"/>
+      <c r="AL19" s="58"/>
+      <c r="AM19" s="58"/>
+      <c r="AN19" s="58"/>
+      <c r="AO19" s="58"/>
+      <c r="AP19" s="58"/>
+      <c r="AQ19" s="60"/>
+      <c r="AR19" s="60"/>
+      <c r="AS19" s="60"/>
+      <c r="AT19" s="60"/>
+      <c r="AU19" s="60"/>
+      <c r="AV19" s="60"/>
     </row>
     <row r="20" spans="37:48" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AQ20" s="5"/>
@@ -6159,52 +6171,52 @@
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="68" t="str">
+      <c r="B2" s="73" t="str">
         <f>Index!$C$10</f>
         <v>Header</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="66" t="str">
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="71" t="str">
         <f>Index!$AB$10</f>
         <v>Project Image</v>
       </c>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="68" t="s">
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="70">
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="75">
         <f>Index!$AK$18</f>
         <v>43955</v>
       </c>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="68" t="s">
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="68"/>
-      <c r="AB2" s="68"/>
-      <c r="AC2" s="66" t="str">
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="71" t="str">
         <f>Index!$AQ$18</f>
         <v>Rick</v>
       </c>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
       <c r="AF2" s="34"/>
       <c r="AG2" s="34"/>
       <c r="AH2" s="34"/>
@@ -6215,36 +6227,36 @@
       <c r="AM2" s="35"/>
     </row>
     <row r="3" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="69"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="71"/>
-      <c r="U3" s="71"/>
-      <c r="V3" s="71"/>
-      <c r="W3" s="71"/>
-      <c r="X3" s="71"/>
-      <c r="Y3" s="71"/>
-      <c r="Z3" s="69"/>
-      <c r="AA3" s="69"/>
-      <c r="AB3" s="69"/>
-      <c r="AC3" s="67"/>
-      <c r="AD3" s="67"/>
-      <c r="AE3" s="67"/>
+      <c r="B3" s="74"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+      <c r="H3" s="74"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
+      <c r="M3" s="72"/>
+      <c r="N3" s="72"/>
+      <c r="O3" s="72"/>
+      <c r="P3" s="74"/>
+      <c r="Q3" s="74"/>
+      <c r="R3" s="74"/>
+      <c r="S3" s="74"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="76"/>
+      <c r="X3" s="76"/>
+      <c r="Y3" s="76"/>
+      <c r="Z3" s="74"/>
+      <c r="AA3" s="74"/>
+      <c r="AB3" s="74"/>
+      <c r="AC3" s="72"/>
+      <c r="AD3" s="72"/>
+      <c r="AE3" s="72"/>
       <c r="AJ3" s="36"/>
       <c r="AK3" s="36"/>
       <c r="AL3" s="36"/>
@@ -6283,52 +6295,52 @@
     </row>
     <row r="5" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35"/>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="78"/>
-      <c r="D5" s="79" t="s">
+      <c r="C5" s="83"/>
+      <c r="D5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="80" t="s">
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-      <c r="L5" s="80"/>
-      <c r="M5" s="80"/>
-      <c r="N5" s="80" t="s">
+      <c r="I5" s="85"/>
+      <c r="J5" s="85"/>
+      <c r="K5" s="85"/>
+      <c r="L5" s="85"/>
+      <c r="M5" s="85"/>
+      <c r="N5" s="85" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="80"/>
-      <c r="P5" s="80"/>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="80"/>
-      <c r="S5" s="80"/>
-      <c r="T5" s="80"/>
-      <c r="U5" s="80"/>
-      <c r="V5" s="80"/>
-      <c r="W5" s="80"/>
-      <c r="X5" s="80"/>
-      <c r="Y5" s="80"/>
-      <c r="Z5" s="80"/>
-      <c r="AA5" s="80"/>
-      <c r="AB5" s="80" t="s">
+      <c r="O5" s="85"/>
+      <c r="P5" s="85"/>
+      <c r="Q5" s="85"/>
+      <c r="R5" s="85"/>
+      <c r="S5" s="85"/>
+      <c r="T5" s="85"/>
+      <c r="U5" s="85"/>
+      <c r="V5" s="85"/>
+      <c r="W5" s="85"/>
+      <c r="X5" s="85"/>
+      <c r="Y5" s="85"/>
+      <c r="Z5" s="85"/>
+      <c r="AA5" s="85"/>
+      <c r="AB5" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="AC5" s="80"/>
-      <c r="AD5" s="80"/>
-      <c r="AE5" s="80"/>
-      <c r="AF5" s="80" t="s">
+      <c r="AC5" s="85"/>
+      <c r="AD5" s="85"/>
+      <c r="AE5" s="85"/>
+      <c r="AF5" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="AG5" s="80"/>
-      <c r="AH5" s="80"/>
-      <c r="AI5" s="81"/>
+      <c r="AG5" s="85"/>
+      <c r="AH5" s="85"/>
+      <c r="AI5" s="86"/>
       <c r="AJ5" s="37"/>
       <c r="AK5" s="37"/>
       <c r="AL5" s="37"/>
@@ -6347,50 +6359,50 @@
     </row>
     <row r="6" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35"/>
-      <c r="B6" s="72">
+      <c r="B6" s="77">
         <v>1</v>
       </c>
-      <c r="C6" s="73"/>
-      <c r="D6" s="74">
+      <c r="C6" s="78"/>
+      <c r="D6" s="79">
         <v>43955</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="75" t="s">
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="75"/>
-      <c r="K6" s="75"/>
-      <c r="L6" s="75"/>
-      <c r="M6" s="75"/>
-      <c r="N6" s="75"/>
-      <c r="O6" s="75"/>
-      <c r="P6" s="75"/>
-      <c r="Q6" s="75"/>
-      <c r="R6" s="75"/>
-      <c r="S6" s="75"/>
-      <c r="T6" s="75"/>
-      <c r="U6" s="75"/>
-      <c r="V6" s="75"/>
-      <c r="W6" s="75"/>
-      <c r="X6" s="75"/>
-      <c r="Y6" s="75"/>
-      <c r="Z6" s="75"/>
-      <c r="AA6" s="75"/>
-      <c r="AB6" s="75" t="s">
+      <c r="I6" s="80"/>
+      <c r="J6" s="80"/>
+      <c r="K6" s="80"/>
+      <c r="L6" s="80"/>
+      <c r="M6" s="80"/>
+      <c r="N6" s="80"/>
+      <c r="O6" s="80"/>
+      <c r="P6" s="80"/>
+      <c r="Q6" s="80"/>
+      <c r="R6" s="80"/>
+      <c r="S6" s="80"/>
+      <c r="T6" s="80"/>
+      <c r="U6" s="80"/>
+      <c r="V6" s="80"/>
+      <c r="W6" s="80"/>
+      <c r="X6" s="80"/>
+      <c r="Y6" s="80"/>
+      <c r="Z6" s="80"/>
+      <c r="AA6" s="80"/>
+      <c r="AB6" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="AC6" s="75"/>
-      <c r="AD6" s="75"/>
-      <c r="AE6" s="75"/>
-      <c r="AF6" s="75" t="s">
+      <c r="AC6" s="80"/>
+      <c r="AD6" s="80"/>
+      <c r="AE6" s="80"/>
+      <c r="AF6" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="AG6" s="75"/>
-      <c r="AH6" s="75"/>
-      <c r="AI6" s="76"/>
+      <c r="AG6" s="80"/>
+      <c r="AH6" s="80"/>
+      <c r="AI6" s="81"/>
       <c r="AJ6" s="37"/>
       <c r="AL6" s="36"/>
       <c r="AM6" s="36"/>
@@ -6407,42 +6419,42 @@
     </row>
     <row r="7" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35"/>
-      <c r="B7" s="82">
+      <c r="B7" s="87">
         <v>2</v>
       </c>
-      <c r="C7" s="83"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="85"/>
-      <c r="I7" s="85"/>
-      <c r="J7" s="85"/>
-      <c r="K7" s="85"/>
-      <c r="L7" s="85"/>
-      <c r="M7" s="85"/>
-      <c r="N7" s="85"/>
-      <c r="O7" s="85"/>
-      <c r="P7" s="85"/>
-      <c r="Q7" s="85"/>
-      <c r="R7" s="85"/>
-      <c r="S7" s="85"/>
-      <c r="T7" s="85"/>
-      <c r="U7" s="85"/>
-      <c r="V7" s="85"/>
-      <c r="W7" s="85"/>
-      <c r="X7" s="85"/>
-      <c r="Y7" s="85"/>
-      <c r="Z7" s="85"/>
-      <c r="AA7" s="85"/>
-      <c r="AB7" s="85"/>
-      <c r="AC7" s="85"/>
-      <c r="AD7" s="85"/>
-      <c r="AE7" s="85"/>
-      <c r="AF7" s="85"/>
-      <c r="AG7" s="85"/>
-      <c r="AH7" s="85"/>
-      <c r="AI7" s="86"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="89"/>
+      <c r="G7" s="89"/>
+      <c r="H7" s="90"/>
+      <c r="I7" s="90"/>
+      <c r="J7" s="90"/>
+      <c r="K7" s="90"/>
+      <c r="L7" s="90"/>
+      <c r="M7" s="90"/>
+      <c r="N7" s="90"/>
+      <c r="O7" s="90"/>
+      <c r="P7" s="90"/>
+      <c r="Q7" s="90"/>
+      <c r="R7" s="90"/>
+      <c r="S7" s="90"/>
+      <c r="T7" s="90"/>
+      <c r="U7" s="90"/>
+      <c r="V7" s="90"/>
+      <c r="W7" s="90"/>
+      <c r="X7" s="90"/>
+      <c r="Y7" s="90"/>
+      <c r="Z7" s="90"/>
+      <c r="AA7" s="90"/>
+      <c r="AB7" s="90"/>
+      <c r="AC7" s="90"/>
+      <c r="AD7" s="90"/>
+      <c r="AE7" s="90"/>
+      <c r="AF7" s="90"/>
+      <c r="AG7" s="90"/>
+      <c r="AH7" s="90"/>
+      <c r="AI7" s="91"/>
       <c r="AJ7" s="37"/>
       <c r="AK7" s="37"/>
       <c r="AL7" s="37"/>
@@ -6461,42 +6473,42 @@
     </row>
     <row r="8" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35"/>
-      <c r="B8" s="82">
+      <c r="B8" s="87">
         <v>3</v>
       </c>
-      <c r="C8" s="83"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="85"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="85"/>
-      <c r="K8" s="85"/>
-      <c r="L8" s="85"/>
-      <c r="M8" s="85"/>
-      <c r="N8" s="85"/>
-      <c r="O8" s="85"/>
-      <c r="P8" s="85"/>
-      <c r="Q8" s="85"/>
-      <c r="R8" s="85"/>
-      <c r="S8" s="85"/>
-      <c r="T8" s="85"/>
-      <c r="U8" s="85"/>
-      <c r="V8" s="85"/>
-      <c r="W8" s="85"/>
-      <c r="X8" s="85"/>
-      <c r="Y8" s="85"/>
-      <c r="Z8" s="85"/>
-      <c r="AA8" s="85"/>
-      <c r="AB8" s="85"/>
-      <c r="AC8" s="85"/>
-      <c r="AD8" s="85"/>
-      <c r="AE8" s="85"/>
-      <c r="AF8" s="85"/>
-      <c r="AG8" s="85"/>
-      <c r="AH8" s="85"/>
-      <c r="AI8" s="86"/>
+      <c r="C8" s="88"/>
+      <c r="D8" s="89"/>
+      <c r="E8" s="89"/>
+      <c r="F8" s="89"/>
+      <c r="G8" s="89"/>
+      <c r="H8" s="90"/>
+      <c r="I8" s="90"/>
+      <c r="J8" s="90"/>
+      <c r="K8" s="90"/>
+      <c r="L8" s="90"/>
+      <c r="M8" s="90"/>
+      <c r="N8" s="90"/>
+      <c r="O8" s="90"/>
+      <c r="P8" s="90"/>
+      <c r="Q8" s="90"/>
+      <c r="R8" s="90"/>
+      <c r="S8" s="90"/>
+      <c r="T8" s="90"/>
+      <c r="U8" s="90"/>
+      <c r="V8" s="90"/>
+      <c r="W8" s="90"/>
+      <c r="X8" s="90"/>
+      <c r="Y8" s="90"/>
+      <c r="Z8" s="90"/>
+      <c r="AA8" s="90"/>
+      <c r="AB8" s="90"/>
+      <c r="AC8" s="90"/>
+      <c r="AD8" s="90"/>
+      <c r="AE8" s="90"/>
+      <c r="AF8" s="90"/>
+      <c r="AG8" s="90"/>
+      <c r="AH8" s="90"/>
+      <c r="AI8" s="91"/>
       <c r="AJ8" s="37"/>
       <c r="AK8" s="37"/>
       <c r="AL8" s="37"/>
@@ -6515,42 +6527,42 @@
     </row>
     <row r="9" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35"/>
-      <c r="B9" s="82">
+      <c r="B9" s="87">
         <v>4</v>
       </c>
-      <c r="C9" s="83"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="85"/>
-      <c r="R9" s="85"/>
-      <c r="S9" s="85"/>
-      <c r="T9" s="85"/>
-      <c r="U9" s="85"/>
-      <c r="V9" s="85"/>
-      <c r="W9" s="85"/>
-      <c r="X9" s="85"/>
-      <c r="Y9" s="85"/>
-      <c r="Z9" s="85"/>
-      <c r="AA9" s="85"/>
-      <c r="AB9" s="85"/>
-      <c r="AC9" s="85"/>
-      <c r="AD9" s="85"/>
-      <c r="AE9" s="85"/>
-      <c r="AF9" s="85"/>
-      <c r="AG9" s="85"/>
-      <c r="AH9" s="85"/>
-      <c r="AI9" s="86"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="89"/>
+      <c r="E9" s="89"/>
+      <c r="F9" s="89"/>
+      <c r="G9" s="89"/>
+      <c r="H9" s="90"/>
+      <c r="I9" s="90"/>
+      <c r="J9" s="90"/>
+      <c r="K9" s="90"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
+      <c r="N9" s="90"/>
+      <c r="O9" s="90"/>
+      <c r="P9" s="90"/>
+      <c r="Q9" s="90"/>
+      <c r="R9" s="90"/>
+      <c r="S9" s="90"/>
+      <c r="T9" s="90"/>
+      <c r="U9" s="90"/>
+      <c r="V9" s="90"/>
+      <c r="W9" s="90"/>
+      <c r="X9" s="90"/>
+      <c r="Y9" s="90"/>
+      <c r="Z9" s="90"/>
+      <c r="AA9" s="90"/>
+      <c r="AB9" s="90"/>
+      <c r="AC9" s="90"/>
+      <c r="AD9" s="90"/>
+      <c r="AE9" s="90"/>
+      <c r="AF9" s="90"/>
+      <c r="AG9" s="90"/>
+      <c r="AH9" s="90"/>
+      <c r="AI9" s="91"/>
       <c r="AJ9" s="37"/>
       <c r="AK9" s="37"/>
       <c r="AL9" s="37"/>
@@ -6569,42 +6581,42 @@
     </row>
     <row r="10" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35"/>
-      <c r="B10" s="87">
+      <c r="B10" s="92">
         <v>5</v>
       </c>
-      <c r="C10" s="88"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="89"/>
-      <c r="F10" s="89"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="90"/>
-      <c r="I10" s="90"/>
-      <c r="J10" s="90"/>
-      <c r="K10" s="90"/>
-      <c r="L10" s="90"/>
-      <c r="M10" s="90"/>
-      <c r="N10" s="90"/>
-      <c r="O10" s="90"/>
-      <c r="P10" s="90"/>
-      <c r="Q10" s="90"/>
-      <c r="R10" s="90"/>
-      <c r="S10" s="90"/>
-      <c r="T10" s="90"/>
-      <c r="U10" s="90"/>
-      <c r="V10" s="90"/>
-      <c r="W10" s="90"/>
-      <c r="X10" s="90"/>
-      <c r="Y10" s="90"/>
-      <c r="Z10" s="90"/>
-      <c r="AA10" s="90"/>
-      <c r="AB10" s="90"/>
-      <c r="AC10" s="90"/>
-      <c r="AD10" s="90"/>
-      <c r="AE10" s="90"/>
-      <c r="AF10" s="90"/>
-      <c r="AG10" s="90"/>
-      <c r="AH10" s="90"/>
-      <c r="AI10" s="91"/>
+      <c r="C10" s="93"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="94"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="94"/>
+      <c r="H10" s="95"/>
+      <c r="I10" s="95"/>
+      <c r="J10" s="95"/>
+      <c r="K10" s="95"/>
+      <c r="L10" s="95"/>
+      <c r="M10" s="95"/>
+      <c r="N10" s="95"/>
+      <c r="O10" s="95"/>
+      <c r="P10" s="95"/>
+      <c r="Q10" s="95"/>
+      <c r="R10" s="95"/>
+      <c r="S10" s="95"/>
+      <c r="T10" s="95"/>
+      <c r="U10" s="95"/>
+      <c r="V10" s="95"/>
+      <c r="W10" s="95"/>
+      <c r="X10" s="95"/>
+      <c r="Y10" s="95"/>
+      <c r="Z10" s="95"/>
+      <c r="AA10" s="95"/>
+      <c r="AB10" s="95"/>
+      <c r="AC10" s="95"/>
+      <c r="AD10" s="95"/>
+      <c r="AE10" s="95"/>
+      <c r="AF10" s="95"/>
+      <c r="AG10" s="95"/>
+      <c r="AH10" s="95"/>
+      <c r="AI10" s="96"/>
       <c r="AJ10" s="38"/>
       <c r="AK10" s="38"/>
       <c r="AL10" s="38"/>
@@ -7084,107 +7096,107 @@
   <sheetData>
     <row r="1" spans="2:88" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="68" t="str">
+      <c r="B2" s="73" t="str">
         <f>Index!$C$10</f>
         <v>Header</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="66" t="str">
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="71" t="str">
         <f>Index!$AB$10</f>
         <v>Project Image</v>
       </c>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="68" t="s">
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="70">
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="75">
         <f>Index!$AK$18</f>
         <v>43955</v>
       </c>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="68" t="s">
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="68"/>
-      <c r="AB2" s="68"/>
-      <c r="AC2" s="66" t="str">
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="71" t="str">
         <f>Index!$AQ$18</f>
         <v>Rick</v>
       </c>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
     </row>
     <row r="3" spans="2:88" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="92"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="92"/>
-      <c r="AB3" s="92"/>
-      <c r="AC3" s="93"/>
-      <c r="AD3" s="93"/>
-      <c r="AE3" s="93"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="97"/>
+      <c r="AA3" s="97"/>
+      <c r="AB3" s="97"/>
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="98"/>
+      <c r="AE3" s="98"/>
     </row>
     <row r="4" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="94" t="s">
+      <c r="B4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="95" t="s">
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="94" t="s">
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="94"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
       <c r="Q4" s="49"/>
       <c r="R4" s="49"/>
       <c r="S4" s="49"/>
@@ -7202,21 +7214,21 @@
       <c r="AE4" s="48"/>
     </row>
     <row r="5" spans="2:88" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
       <c r="Q5" s="44"/>
       <c r="R5" s="44"/>
       <c r="S5" s="44"/>
@@ -7280,7 +7292,7 @@
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
-      <c r="R7" s="96"/>
+      <c r="R7" s="52"/>
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
       <c r="U7" s="15"/>
@@ -7623,39 +7635,39 @@
       <c r="C11" s="5"/>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
-      <c r="H11" s="97"/>
-      <c r="I11" s="97"/>
-      <c r="J11" s="97"/>
-      <c r="K11" s="97"/>
-      <c r="L11" s="97"/>
-      <c r="M11" s="97"/>
-      <c r="N11" s="97"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
+      <c r="N11" s="53"/>
       <c r="O11" s="5"/>
-      <c r="P11" s="98"/>
-      <c r="Q11" s="98"/>
-      <c r="R11" s="98"/>
-      <c r="S11" s="98"/>
-      <c r="T11" s="98"/>
-      <c r="U11" s="98"/>
-      <c r="V11" s="98"/>
-      <c r="W11" s="98"/>
-      <c r="X11" s="98"/>
-      <c r="Y11" s="98"/>
-      <c r="Z11" s="98"/>
-      <c r="AA11" s="98"/>
-      <c r="AB11" s="98"/>
-      <c r="AC11" s="98"/>
-      <c r="AD11" s="98"/>
-      <c r="AE11" s="98"/>
-      <c r="AF11" s="98"/>
-      <c r="AG11" s="98"/>
-      <c r="AH11" s="98"/>
-      <c r="AI11" s="98"/>
-      <c r="AJ11" s="98"/>
-      <c r="AK11" s="98"/>
-      <c r="AL11" s="98"/>
-      <c r="AM11" s="98"/>
-      <c r="AN11" s="98"/>
+      <c r="P11" s="54"/>
+      <c r="Q11" s="54"/>
+      <c r="R11" s="54"/>
+      <c r="S11" s="54"/>
+      <c r="T11" s="54"/>
+      <c r="U11" s="54"/>
+      <c r="V11" s="54"/>
+      <c r="W11" s="54"/>
+      <c r="X11" s="54"/>
+      <c r="Y11" s="54"/>
+      <c r="Z11" s="54"/>
+      <c r="AA11" s="54"/>
+      <c r="AB11" s="54"/>
+      <c r="AC11" s="54"/>
+      <c r="AD11" s="54"/>
+      <c r="AE11" s="54"/>
+      <c r="AF11" s="54"/>
+      <c r="AG11" s="54"/>
+      <c r="AH11" s="54"/>
+      <c r="AI11" s="54"/>
+      <c r="AJ11" s="54"/>
+      <c r="AK11" s="54"/>
+      <c r="AL11" s="54"/>
+      <c r="AM11" s="54"/>
+      <c r="AN11" s="54"/>
       <c r="AO11" s="5"/>
       <c r="AP11" s="5"/>
       <c r="AQ11" s="5"/>
@@ -10709,11 +10721,11 @@
     <tabColor theme="5" tint="0.79998168889431442"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:CJ45"/>
+  <dimension ref="B1:CJ48"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="3" style="1"/>
     <col min="3" max="3" width="2.88671875" style="2" customWidth="1"/>
@@ -10723,109 +10735,109 @@
     <col min="9" max="16384" width="3" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:88" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="68" t="str">
+    <row r="1" spans="2:88" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="73" t="str">
         <f>Index!$C$10</f>
         <v>Header</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
-      <c r="H2" s="68"/>
-      <c r="I2" s="66" t="str">
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="71" t="str">
         <f>Index!$AB$10</f>
         <v>Project Image</v>
       </c>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
-      <c r="L2" s="66"/>
-      <c r="M2" s="66"/>
-      <c r="N2" s="66"/>
-      <c r="O2" s="66"/>
-      <c r="P2" s="68" t="s">
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="71"/>
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="68"/>
-      <c r="T2" s="70">
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="75">
         <f>Index!$AK$18</f>
         <v>43955</v>
       </c>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="68" t="s">
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="68"/>
-      <c r="AB2" s="68"/>
-      <c r="AC2" s="66" t="str">
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="71" t="str">
         <f>Index!$AQ$18</f>
         <v>Rick</v>
       </c>
-      <c r="AD2" s="66"/>
-      <c r="AE2" s="66"/>
+      <c r="AD2" s="71"/>
+      <c r="AE2" s="71"/>
     </row>
-    <row r="3" spans="2:88" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="92"/>
-      <c r="C3" s="92"/>
-      <c r="D3" s="92"/>
-      <c r="E3" s="92"/>
-      <c r="F3" s="92"/>
-      <c r="G3" s="92"/>
-      <c r="H3" s="92"/>
-      <c r="I3" s="93"/>
-      <c r="J3" s="93"/>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="92"/>
-      <c r="Q3" s="92"/>
-      <c r="R3" s="92"/>
-      <c r="S3" s="92"/>
-      <c r="T3" s="53"/>
-      <c r="U3" s="53"/>
-      <c r="V3" s="53"/>
-      <c r="W3" s="53"/>
-      <c r="X3" s="53"/>
-      <c r="Y3" s="53"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="92"/>
-      <c r="AB3" s="92"/>
-      <c r="AC3" s="93"/>
-      <c r="AD3" s="93"/>
-      <c r="AE3" s="93"/>
+    <row r="3" spans="2:88" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="97"/>
+      <c r="C3" s="97"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
+      <c r="H3" s="97"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="98"/>
+      <c r="L3" s="98"/>
+      <c r="M3" s="98"/>
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="97"/>
+      <c r="Q3" s="97"/>
+      <c r="R3" s="97"/>
+      <c r="S3" s="97"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="97"/>
+      <c r="AA3" s="97"/>
+      <c r="AB3" s="97"/>
+      <c r="AC3" s="98"/>
+      <c r="AD3" s="98"/>
+      <c r="AE3" s="98"/>
     </row>
-    <row r="4" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="94" t="s">
+    <row r="4" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="95" t="s">
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="100" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="94" t="s">
+      <c r="H4" s="100"/>
+      <c r="I4" s="100"/>
+      <c r="J4" s="100"/>
+      <c r="K4" s="100"/>
+      <c r="L4" s="100"/>
+      <c r="M4" s="99" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="94"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="99"/>
+      <c r="P4" s="99"/>
       <c r="Q4" s="49"/>
       <c r="R4" s="49"/>
       <c r="S4" s="49"/>
@@ -10842,22 +10854,22 @@
       <c r="AD4" s="48"/>
       <c r="AE4" s="48"/>
     </row>
-    <row r="5" spans="2:88" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="69"/>
-      <c r="C5" s="69"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67"/>
-      <c r="I5" s="67"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="67"/>
-      <c r="L5" s="67"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
+    <row r="5" spans="2:88" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="74"/>
+      <c r="N5" s="74"/>
+      <c r="O5" s="74"/>
+      <c r="P5" s="74"/>
       <c r="Q5" s="44"/>
       <c r="R5" s="44"/>
       <c r="S5" s="44"/>
@@ -10874,7 +10886,7 @@
       <c r="AD5" s="45"/>
       <c r="AE5" s="45"/>
     </row>
-    <row r="6" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="L6" s="11"/>
       <c r="M6" s="11"/>
       <c r="N6" s="11"/>
@@ -10904,7 +10916,7 @@
       <c r="AL6" s="11"/>
       <c r="AM6" s="14"/>
     </row>
-    <row r="7" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
@@ -10921,7 +10933,7 @@
       <c r="O7" s="15"/>
       <c r="P7" s="15"/>
       <c r="Q7" s="15"/>
-      <c r="R7" s="96"/>
+      <c r="R7" s="52"/>
       <c r="S7" s="15"/>
       <c r="T7" s="15"/>
       <c r="U7" s="15"/>
@@ -10993,9 +11005,9 @@
       <c r="CI7" s="5"/>
       <c r="CJ7" s="5"/>
     </row>
-    <row r="8" spans="2:88" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
-      <c r="C8" s="100" t="s">
+      <c r="C8" s="56" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="25"/>
@@ -11084,7 +11096,7 @@
       <c r="CI8" s="5"/>
       <c r="CJ8" s="5"/>
     </row>
-    <row r="9" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -11172,44 +11184,44 @@
       <c r="CI9" s="5"/>
       <c r="CJ9" s="5"/>
     </row>
-    <row r="10" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
-      <c r="H10" s="97"/>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
-      <c r="K10" s="97"/>
-      <c r="L10" s="97"/>
-      <c r="M10" s="97"/>
-      <c r="N10" s="97"/>
+      <c r="H10" s="53"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="53"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="53"/>
+      <c r="N10" s="53"/>
       <c r="O10" s="5"/>
-      <c r="P10" s="98"/>
-      <c r="Q10" s="98"/>
-      <c r="R10" s="98"/>
-      <c r="S10" s="98"/>
-      <c r="T10" s="98"/>
-      <c r="U10" s="98"/>
-      <c r="V10" s="98"/>
-      <c r="W10" s="98"/>
-      <c r="X10" s="98"/>
-      <c r="Y10" s="98"/>
-      <c r="Z10" s="98"/>
-      <c r="AA10" s="98"/>
-      <c r="AB10" s="98"/>
-      <c r="AC10" s="98"/>
-      <c r="AD10" s="98"/>
-      <c r="AE10" s="98"/>
-      <c r="AF10" s="98"/>
-      <c r="AG10" s="98"/>
-      <c r="AH10" s="98"/>
-      <c r="AI10" s="98"/>
-      <c r="AJ10" s="98"/>
-      <c r="AK10" s="98"/>
-      <c r="AL10" s="98"/>
-      <c r="AM10" s="98"/>
-      <c r="AN10" s="98"/>
+      <c r="P10" s="54"/>
+      <c r="Q10" s="54"/>
+      <c r="R10" s="54"/>
+      <c r="S10" s="54"/>
+      <c r="T10" s="54"/>
+      <c r="U10" s="54"/>
+      <c r="V10" s="54"/>
+      <c r="W10" s="54"/>
+      <c r="X10" s="54"/>
+      <c r="Y10" s="54"/>
+      <c r="Z10" s="54"/>
+      <c r="AA10" s="54"/>
+      <c r="AB10" s="54"/>
+      <c r="AC10" s="54"/>
+      <c r="AD10" s="54"/>
+      <c r="AE10" s="54"/>
+      <c r="AF10" s="54"/>
+      <c r="AG10" s="54"/>
+      <c r="AH10" s="54"/>
+      <c r="AI10" s="54"/>
+      <c r="AJ10" s="54"/>
+      <c r="AK10" s="54"/>
+      <c r="AL10" s="54"/>
+      <c r="AM10" s="54"/>
+      <c r="AN10" s="54"/>
       <c r="AO10" s="5"/>
       <c r="AP10" s="5"/>
       <c r="AQ10" s="5"/>
@@ -11259,11 +11271,11 @@
       <c r="CI10" s="5"/>
       <c r="CJ10" s="5"/>
     </row>
-    <row r="11" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="99"/>
+      <c r="E11" s="55"/>
       <c r="F11" s="5"/>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
@@ -11347,7 +11359,7 @@
       <c r="CI11" s="5"/>
       <c r="CJ11" s="5"/>
     </row>
-    <row r="12" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
       <c r="D12" s="26"/>
@@ -11436,7 +11448,7 @@
       <c r="CI12" s="5"/>
       <c r="CJ12" s="5"/>
     </row>
-    <row r="13" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
       <c r="D13" s="26"/>
@@ -11525,7 +11537,7 @@
       <c r="CI13" s="5"/>
       <c r="CJ13" s="5"/>
     </row>
-    <row r="14" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
       <c r="D14" s="26"/>
@@ -11614,7 +11626,7 @@
       <c r="CI14" s="5"/>
       <c r="CJ14" s="5"/>
     </row>
-    <row r="15" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22"/>
@@ -11703,7 +11715,7 @@
       <c r="CI15" s="5"/>
       <c r="CJ15" s="5"/>
     </row>
-    <row r="16" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="22"/>
       <c r="C16" s="22"/>
       <c r="F16" s="24"/>
@@ -11790,7 +11802,7 @@
       <c r="CI16" s="5"/>
       <c r="CJ16" s="5"/>
     </row>
-    <row r="17" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="22"/>
       <c r="C17" s="22"/>
       <c r="F17" s="24"/>
@@ -11877,7 +11889,7 @@
       <c r="CI17" s="5"/>
       <c r="CJ17" s="5"/>
     </row>
-    <row r="18" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="I18" s="5"/>
@@ -11961,7 +11973,7 @@
       <c r="CI18" s="5"/>
       <c r="CJ18" s="5"/>
     </row>
-    <row r="19" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="I19" s="5"/>
@@ -12045,7 +12057,7 @@
       <c r="CI19" s="5"/>
       <c r="CJ19" s="5"/>
     </row>
-    <row r="20" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="I20" s="5"/>
@@ -12129,7 +12141,7 @@
       <c r="CI20" s="5"/>
       <c r="CJ20" s="5"/>
     </row>
-    <row r="21" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="I21" s="5"/>
@@ -12213,7 +12225,7 @@
       <c r="CI21" s="5"/>
       <c r="CJ21" s="5"/>
     </row>
-    <row r="22" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="I22" s="5"/>
@@ -12297,7 +12309,7 @@
       <c r="CI22" s="5"/>
       <c r="CJ22" s="5"/>
     </row>
-    <row r="23" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="I23" s="5"/>
@@ -12381,7 +12393,7 @@
       <c r="CI23" s="5"/>
       <c r="CJ23" s="5"/>
     </row>
-    <row r="24" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="I24" s="5"/>
@@ -12465,7 +12477,7 @@
       <c r="CI24" s="5"/>
       <c r="CJ24" s="5"/>
     </row>
-    <row r="25" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="I25" s="5"/>
@@ -12549,7 +12561,7 @@
       <c r="CI25" s="5"/>
       <c r="CJ25" s="5"/>
     </row>
-    <row r="26" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="I26" s="5"/>
@@ -12633,7 +12645,7 @@
       <c r="CI26" s="5"/>
       <c r="CJ26" s="5"/>
     </row>
-    <row r="27" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="I27" s="5"/>
@@ -12717,7 +12729,7 @@
       <c r="CI27" s="5"/>
       <c r="CJ27" s="5"/>
     </row>
-    <row r="28" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="I28" s="5"/>
@@ -12801,7 +12813,7 @@
       <c r="CI28" s="5"/>
       <c r="CJ28" s="5"/>
     </row>
-    <row r="29" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="I29" s="5"/>
@@ -12885,9 +12897,9 @@
       <c r="CI29" s="5"/>
       <c r="CJ29" s="5"/>
     </row>
-    <row r="30" spans="2:88" ht="26.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
-      <c r="C30" s="100" t="s">
+      <c r="C30" s="56" t="s">
         <v>16</v>
       </c>
       <c r="D30" s="25"/>
@@ -12976,7 +12988,7 @@
       <c r="CI30" s="5"/>
       <c r="CJ30" s="5"/>
     </row>
-    <row r="31" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="I31" s="5"/>
@@ -13060,7 +13072,7 @@
       <c r="CI31" s="5"/>
       <c r="CJ31" s="5"/>
     </row>
-    <row r="32" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="I32" s="5"/>
@@ -13144,7 +13156,7 @@
       <c r="CI32" s="5"/>
       <c r="CJ32" s="5"/>
     </row>
-    <row r="33" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="I33" s="5"/>
@@ -13228,7 +13240,7 @@
       <c r="CI33" s="5"/>
       <c r="CJ33" s="5"/>
     </row>
-    <row r="34" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="I34" s="5"/>
@@ -13312,11 +13324,18 @@
       <c r="CI34" s="5"/>
       <c r="CJ34" s="5"/>
     </row>
-    <row r="35" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
+      <c r="D35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
@@ -13396,7 +13415,7 @@
       <c r="CI35" s="5"/>
       <c r="CJ35" s="5"/>
     </row>
-    <row r="36" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="I36" s="5"/>
@@ -13480,7 +13499,7 @@
       <c r="CI36" s="5"/>
       <c r="CJ36" s="5"/>
     </row>
-    <row r="37" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="I37" s="5"/>
@@ -13564,7 +13583,7 @@
       <c r="CI37" s="5"/>
       <c r="CJ37" s="5"/>
     </row>
-    <row r="38" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="I38" s="5"/>
@@ -13648,7 +13667,7 @@
       <c r="CI38" s="5"/>
       <c r="CJ38" s="5"/>
     </row>
-    <row r="39" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="I39" s="5"/>
@@ -13732,7 +13751,7 @@
       <c r="CI39" s="5"/>
       <c r="CJ39" s="5"/>
     </row>
-    <row r="40" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="I40" s="5"/>
@@ -13816,7 +13835,7 @@
       <c r="CI40" s="5"/>
       <c r="CJ40" s="5"/>
     </row>
-    <row r="41" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="I41" s="5"/>
@@ -13900,7 +13919,7 @@
       <c r="CI41" s="5"/>
       <c r="CJ41" s="5"/>
     </row>
-    <row r="42" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="I42" s="5"/>
@@ -13984,7 +14003,7 @@
       <c r="CI42" s="5"/>
       <c r="CJ42" s="5"/>
     </row>
-    <row r="43" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="I43" s="5"/>
@@ -14068,7 +14087,7 @@
       <c r="CI43" s="5"/>
       <c r="CJ43" s="5"/>
     </row>
-    <row r="44" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="I44" s="5"/>
@@ -14152,7 +14171,7 @@
       <c r="CI44" s="5"/>
       <c r="CJ44" s="5"/>
     </row>
-    <row r="45" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="I45" s="5"/>
@@ -14236,17 +14255,269 @@
       <c r="CI45" s="5"/>
       <c r="CJ45" s="5"/>
     </row>
+    <row r="46" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="5"/>
+      <c r="AC46" s="5"/>
+      <c r="AD46" s="5"/>
+      <c r="AE46" s="5"/>
+      <c r="AF46" s="5"/>
+      <c r="AG46" s="5"/>
+      <c r="AH46" s="5"/>
+      <c r="AI46" s="5"/>
+      <c r="AJ46" s="5"/>
+      <c r="AK46" s="5"/>
+      <c r="AL46" s="5"/>
+      <c r="AM46" s="5"/>
+      <c r="AN46" s="5"/>
+      <c r="AO46" s="5"/>
+      <c r="AP46" s="5"/>
+      <c r="AQ46" s="5"/>
+      <c r="AR46" s="5"/>
+      <c r="AS46" s="5"/>
+      <c r="AT46" s="5"/>
+      <c r="AU46" s="5"/>
+      <c r="AV46" s="5"/>
+      <c r="AW46" s="5"/>
+      <c r="AX46" s="5"/>
+      <c r="AY46" s="5"/>
+      <c r="AZ46" s="5"/>
+      <c r="BA46" s="5"/>
+      <c r="BB46" s="5"/>
+      <c r="BC46" s="5"/>
+      <c r="BD46" s="5"/>
+      <c r="BE46" s="5"/>
+      <c r="BF46" s="5"/>
+      <c r="BG46" s="5"/>
+      <c r="BH46" s="5"/>
+      <c r="BI46" s="5"/>
+      <c r="BJ46" s="5"/>
+      <c r="BK46" s="5"/>
+      <c r="BL46" s="5"/>
+      <c r="BM46" s="5"/>
+      <c r="BN46" s="5"/>
+      <c r="BO46" s="5"/>
+      <c r="BP46" s="5"/>
+      <c r="BQ46" s="5"/>
+      <c r="BR46" s="5"/>
+      <c r="BS46" s="5"/>
+      <c r="BT46" s="5"/>
+      <c r="BU46" s="5"/>
+      <c r="BV46" s="5"/>
+      <c r="BW46" s="5"/>
+      <c r="BX46" s="5"/>
+      <c r="BY46" s="5"/>
+      <c r="BZ46" s="5"/>
+      <c r="CA46" s="5"/>
+      <c r="CB46" s="5"/>
+      <c r="CC46" s="5"/>
+      <c r="CD46" s="5"/>
+      <c r="CE46" s="5"/>
+      <c r="CF46" s="5"/>
+      <c r="CG46" s="5"/>
+      <c r="CH46" s="5"/>
+      <c r="CI46" s="5"/>
+      <c r="CJ46" s="5"/>
+    </row>
+    <row r="47" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+      <c r="P47" s="5"/>
+      <c r="Q47" s="5"/>
+      <c r="R47" s="5"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="5"/>
+      <c r="U47" s="5"/>
+      <c r="V47" s="5"/>
+      <c r="W47" s="5"/>
+      <c r="X47" s="5"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5"/>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5"/>
+      <c r="AE47" s="5"/>
+      <c r="AF47" s="5"/>
+      <c r="AG47" s="5"/>
+      <c r="AH47" s="5"/>
+      <c r="AI47" s="5"/>
+      <c r="AJ47" s="5"/>
+      <c r="AK47" s="5"/>
+      <c r="AL47" s="5"/>
+      <c r="AM47" s="5"/>
+      <c r="AN47" s="5"/>
+      <c r="AO47" s="5"/>
+      <c r="AP47" s="5"/>
+      <c r="AQ47" s="5"/>
+      <c r="AR47" s="5"/>
+      <c r="AS47" s="5"/>
+      <c r="AT47" s="5"/>
+      <c r="AU47" s="5"/>
+      <c r="AV47" s="5"/>
+      <c r="AW47" s="5"/>
+      <c r="AX47" s="5"/>
+      <c r="AY47" s="5"/>
+      <c r="AZ47" s="5"/>
+      <c r="BA47" s="5"/>
+      <c r="BB47" s="5"/>
+      <c r="BC47" s="5"/>
+      <c r="BD47" s="5"/>
+      <c r="BE47" s="5"/>
+      <c r="BF47" s="5"/>
+      <c r="BG47" s="5"/>
+      <c r="BH47" s="5"/>
+      <c r="BI47" s="5"/>
+      <c r="BJ47" s="5"/>
+      <c r="BK47" s="5"/>
+      <c r="BL47" s="5"/>
+      <c r="BM47" s="5"/>
+      <c r="BN47" s="5"/>
+      <c r="BO47" s="5"/>
+      <c r="BP47" s="5"/>
+      <c r="BQ47" s="5"/>
+      <c r="BR47" s="5"/>
+      <c r="BS47" s="5"/>
+      <c r="BT47" s="5"/>
+      <c r="BU47" s="5"/>
+      <c r="BV47" s="5"/>
+      <c r="BW47" s="5"/>
+      <c r="BX47" s="5"/>
+      <c r="BY47" s="5"/>
+      <c r="BZ47" s="5"/>
+      <c r="CA47" s="5"/>
+      <c r="CB47" s="5"/>
+      <c r="CC47" s="5"/>
+      <c r="CD47" s="5"/>
+      <c r="CE47" s="5"/>
+      <c r="CF47" s="5"/>
+      <c r="CG47" s="5"/>
+      <c r="CH47" s="5"/>
+      <c r="CI47" s="5"/>
+      <c r="CJ47" s="5"/>
+    </row>
+    <row r="48" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+      <c r="P48" s="5"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5"/>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5"/>
+      <c r="AE48" s="5"/>
+      <c r="AF48" s="5"/>
+      <c r="AG48" s="5"/>
+      <c r="AH48" s="5"/>
+      <c r="AI48" s="5"/>
+      <c r="AJ48" s="5"/>
+      <c r="AK48" s="5"/>
+      <c r="AL48" s="5"/>
+      <c r="AM48" s="5"/>
+      <c r="AN48" s="5"/>
+      <c r="AO48" s="5"/>
+      <c r="AP48" s="5"/>
+      <c r="AQ48" s="5"/>
+      <c r="AR48" s="5"/>
+      <c r="AS48" s="5"/>
+      <c r="AT48" s="5"/>
+      <c r="AU48" s="5"/>
+      <c r="AV48" s="5"/>
+      <c r="AW48" s="5"/>
+      <c r="AX48" s="5"/>
+      <c r="AY48" s="5"/>
+      <c r="AZ48" s="5"/>
+      <c r="BA48" s="5"/>
+      <c r="BB48" s="5"/>
+      <c r="BC48" s="5"/>
+      <c r="BD48" s="5"/>
+      <c r="BE48" s="5"/>
+      <c r="BF48" s="5"/>
+      <c r="BG48" s="5"/>
+      <c r="BH48" s="5"/>
+      <c r="BI48" s="5"/>
+      <c r="BJ48" s="5"/>
+      <c r="BK48" s="5"/>
+      <c r="BL48" s="5"/>
+      <c r="BM48" s="5"/>
+      <c r="BN48" s="5"/>
+      <c r="BO48" s="5"/>
+      <c r="BP48" s="5"/>
+      <c r="BQ48" s="5"/>
+      <c r="BR48" s="5"/>
+      <c r="BS48" s="5"/>
+      <c r="BT48" s="5"/>
+      <c r="BU48" s="5"/>
+      <c r="BV48" s="5"/>
+      <c r="BW48" s="5"/>
+      <c r="BX48" s="5"/>
+      <c r="BY48" s="5"/>
+      <c r="BZ48" s="5"/>
+      <c r="CA48" s="5"/>
+      <c r="CB48" s="5"/>
+      <c r="CC48" s="5"/>
+      <c r="CD48" s="5"/>
+      <c r="CE48" s="5"/>
+      <c r="CF48" s="5"/>
+      <c r="CG48" s="5"/>
+      <c r="CH48" s="5"/>
+      <c r="CI48" s="5"/>
+      <c r="CJ48" s="5"/>
+    </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="T2:Y3"/>
+    <mergeCell ref="Z2:AB3"/>
+    <mergeCell ref="AC2:AE3"/>
     <mergeCell ref="B4:F5"/>
     <mergeCell ref="G4:L5"/>
     <mergeCell ref="M4:P5"/>
     <mergeCell ref="B2:H3"/>
     <mergeCell ref="I2:O3"/>
     <mergeCell ref="P2:S3"/>
-    <mergeCell ref="T2:Y3"/>
-    <mergeCell ref="Z2:AB3"/>
-    <mergeCell ref="AC2:AE3"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Update ParkingArea Project's Documents
</commit_message>
<xml_diff>
--- a/SimpleProjects/Module/ParkingArea/1.Design/Image.xlsx
+++ b/SimpleProjects/Module/ParkingArea/1.Design/Image.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="14955" windowHeight="7500"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="14955" windowHeight="7500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="2" r:id="rId1"/>
@@ -679,54 +679,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -756,6 +708,54 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -860,6 +860,79 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>81642</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>71</xdr:col>
+      <xdr:colOff>258534</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>204106</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="42" name="모서리가 둥근 직사각형 41"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6531428" y="1170215"/>
+          <a:ext cx="12069535" cy="7198177"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 4031"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="40000"/>
+            <a:lumOff val="60000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx2">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="2000" b="1" i="1"/>
+            <a:t>Functions</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="2000" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
@@ -922,592 +995,6 @@
             <a:rPr lang="en-US" altLang="ko-KR" sz="3600" b="1" i="0"/>
             <a:t>Main</a:t>
           </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>73</xdr:col>
-      <xdr:colOff>101653</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>85936</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>84</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>149680</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 17"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="18961153" y="494150"/>
-          <a:ext cx="2742240" cy="2921244"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 9299"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="tx1"/>
-          </a:solidFill>
-          <a:prstDash val="sysDot"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1800" b="1" i="1">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Description</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1800" b="1" i="1" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> for Elements</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1800" b="1" i="1">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>74</xdr:col>
-      <xdr:colOff>101653</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>13608</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>101653</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>13608</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="모서리가 둥근 직사각형 16"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="19219689" y="1034144"/>
-          <a:ext cx="258535" cy="204107"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="sysDot"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1"/>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1" i="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>74</xdr:col>
-      <xdr:colOff>101653</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>173024</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>101653</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>173023</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="직사각형 20"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19219689" y="1397667"/>
-          <a:ext cx="258535" cy="204106"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="95000"/>
-              <a:lumOff val="5000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1600"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>247329</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>161977</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>81</xdr:col>
-      <xdr:colOff>101652</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>190502</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="TextBox 22"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19623900" y="1386620"/>
-          <a:ext cx="1405538" cy="232632"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Method</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>247329</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>189190</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>81</xdr:col>
-      <xdr:colOff>101652</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>13608</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="TextBox 27"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19623900" y="1005619"/>
-          <a:ext cx="1405538" cy="232632"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Function</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>74</xdr:col>
-      <xdr:colOff>101652</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>68168</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>101653</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>68168</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="129" name="모서리가 둥근 직사각형 128"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19219688" y="2313347"/>
-          <a:ext cx="258536" cy="204107"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFF8C"/>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="sysDot"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1" i="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>247329</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>81</xdr:col>
-      <xdr:colOff>99559</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>81907</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="131" name="TextBox 130"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19623900" y="2245179"/>
-          <a:ext cx="1403445" cy="286014"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Inner</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Function</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>247329</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>190501</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>81</xdr:col>
-      <xdr:colOff>99559</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114143</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="86" name="TextBox 85"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19623900" y="1823358"/>
-          <a:ext cx="1403445" cy="331856"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>User</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Input</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1901,14 +1388,14 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
       <xdr:colOff>258535</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1917,8 +1404,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7225393" y="1428750"/>
-          <a:ext cx="3360963" cy="3265714"/>
+          <a:off x="7225393" y="1836964"/>
+          <a:ext cx="3360963" cy="1986644"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
@@ -1978,13 +1465,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>12370</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>163285</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>163284</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
       <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>169099</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1994,7 +1481,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7496299" y="2000249"/>
+          <a:off x="7496299" y="2408463"/>
           <a:ext cx="2668236" cy="414029"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2050,25 +1537,176 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>12370</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>199570</xdr:rowOff>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>1278</xdr:rowOff>
+      <xdr:col>56</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="98" name="직사각형 97"/>
+        <xdr:cNvPr id="104" name="모서리가 둥근 직사각형 103"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7496299" y="2648856"/>
+          <a:off x="11117036" y="1836964"/>
+          <a:ext cx="3360964" cy="2653393"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 8568"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent4">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="dash"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1"/>
+            <a:t>Function 2)</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1" baseline="0"/>
+            <a:t> Exit car from parking area</a:t>
+          </a:r>
+          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>202869</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>40821</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>27212</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>46636</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="105" name="직사각형 104"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11564833" y="3102428"/>
+          <a:ext cx="2668236" cy="414029"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
+            <a:t>Estimate</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1" baseline="0"/>
+            <a:t> cost</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>202869</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>197303</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>27212</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>203118</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="107" name="직사각형 106"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11564833" y="2442482"/>
           <a:ext cx="2668236" cy="414029"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2138,530 +1776,14 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>12370</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>31749</xdr:rowOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>204104</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>39</xdr:col>
       <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>37563</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="99" name="직사각형 98"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7496299" y="3297463"/>
-          <a:ext cx="2668236" cy="414029"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="95000"/>
-              <a:lumOff val="5000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
-            <a:t>Regist</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1" baseline="0"/>
-            <a:t> Data</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>74</xdr:col>
-      <xdr:colOff>88046</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>142475</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="101" name="타원 100"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19206082" y="2748643"/>
-          <a:ext cx="312964" cy="312964"/>
-        </a:xfrm>
-        <a:prstGeom prst="ellipse">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="90000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>247329</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>190500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>81</xdr:col>
-      <xdr:colOff>99559</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>109122</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="102" name="TextBox 101"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="19623900" y="2639786"/>
-          <a:ext cx="1403445" cy="530943"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="bg2">
-            <a:lumMod val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="9525" cmpd="sng">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
-              <a:solidFill>
-                <a:schemeClr val="bg1"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Function Executer</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
-            <a:solidFill>
-              <a:schemeClr val="bg1"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>57</xdr:col>
-      <xdr:colOff>-1</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="104" name="모서리가 둥근 직사각형 103"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11361964" y="1428750"/>
-          <a:ext cx="3360964" cy="3265715"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 8568"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent4">
-              <a:lumMod val="40000"/>
-              <a:lumOff val="60000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="dash"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1"/>
-            <a:t>Function 2)</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1" baseline="0"/>
-            <a:t> Exit car from parking area</a:t>
-          </a:r>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1" i="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>189261</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>40821</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>13604</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>46636</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="105" name="직사각형 104"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11809761" y="2694214"/>
-          <a:ext cx="2668236" cy="414029"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="95000"/>
-              <a:lumOff val="5000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
-            <a:t>Estimate</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1" baseline="0"/>
-            <a:t> cost</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>189261</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>197304</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>13604</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>203118</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="107" name="직사각형 106"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11809761" y="2034268"/>
-          <a:ext cx="2668236" cy="414029"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="95000"/>
-              <a:lumOff val="5000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>(TODO)Check</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF0000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Member</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1">
-            <a:solidFill>
-              <a:srgbClr val="FF0000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>189261</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>88446</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>13604</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>94260</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="113" name="직사각형 112"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11809761" y="3354160"/>
-          <a:ext cx="2668236" cy="414029"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent4">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="tx1">
-              <a:lumMod val="95000"/>
-              <a:lumOff val="5000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
-            <a:t>Update Data</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>12370</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>68034</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>73849</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>5812</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2670,7 +1792,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7496299" y="3946070"/>
+          <a:off x="7496299" y="3061604"/>
           <a:ext cx="2668236" cy="414029"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2726,16 +1848,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>45</xdr:col>
-      <xdr:colOff>189261</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>136071</xdr:rowOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>202869</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>56</xdr:col>
-      <xdr:colOff>13604</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>141886</xdr:rowOff>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>27212</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>101064</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2744,7 +1866,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11809761" y="4014107"/>
+          <a:off x="11564833" y="3769178"/>
           <a:ext cx="2668236" cy="414029"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2801,15 +1923,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>58</xdr:col>
-      <xdr:colOff>149679</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:colOff>122465</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>71</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2818,7 +1940,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15131143" y="1428751"/>
+          <a:off x="15103929" y="1836964"/>
           <a:ext cx="3238500" cy="1387928"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -2878,15 +2000,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>59</xdr:col>
-      <xdr:colOff>175657</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>198293</xdr:rowOff>
+      <xdr:colOff>148443</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>198291</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>70</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>69</xdr:col>
+      <xdr:colOff>231322</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>204106</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2895,7 +2017,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15415657" y="2035257"/>
+          <a:off x="15388443" y="2443470"/>
           <a:ext cx="2668236" cy="414029"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3014,7 +2136,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1"/>
-            <a:t>Function 5)</a:t>
+            <a:t>Function 4)</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1" baseline="0"/>
@@ -3162,7 +2284,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
-            <a:t>Ouput</a:t>
+            <a:t>Output</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1" baseline="0"/>
@@ -3546,71 +2668,637 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>74</xdr:col>
-      <xdr:colOff>88046</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>27215</xdr:rowOff>
+      <xdr:col>73</xdr:col>
+      <xdr:colOff>101653</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>140363</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>128869</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>27215</xdr:rowOff>
+      <xdr:col>84</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="139" name="모서리가 둥근 직사각형 138"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="3" name="그룹 2"/>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="19206082" y="1864179"/>
-          <a:ext cx="299358" cy="204107"/>
+          <a:off x="18961153" y="1160899"/>
+          <a:ext cx="2742240" cy="2921244"/>
+          <a:chOff x="18961153" y="1160899"/>
+          <a:chExt cx="2742240" cy="2921244"/>
         </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent3">
-            <a:lumMod val="40000"/>
-            <a:lumOff val="60000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="28575">
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="18" name="모서리가 둥근 직사각형 17"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="18961153" y="1160899"/>
+            <a:ext cx="2742240" cy="2921244"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 9299"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1800" b="1" i="1">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Description</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1800" b="1" i="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> for Elements</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1800" b="1" i="1">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="17" name="모서리가 둥근 직사각형 16"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm rot="10800000" flipV="1">
+            <a:off x="19219689" y="1700893"/>
+            <a:ext cx="258535" cy="204107"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1"/>
+          </a:p>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1" i="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="21" name="직사각형 20"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19219689" y="2064416"/>
+            <a:ext cx="258535" cy="204106"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
           <a:solidFill>
             <a:schemeClr val="accent4">
+              <a:lumMod val="20000"/>
+              <a:lumOff val="80000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1600"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="TextBox 22"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19623900" y="2053369"/>
+            <a:ext cx="1405538" cy="232632"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Method</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="28" name="TextBox 27"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19623900" y="1672368"/>
+            <a:ext cx="1405538" cy="232632"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Function</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="129" name="모서리가 둥근 직사각형 128"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19219688" y="2980096"/>
+            <a:ext cx="258536" cy="204107"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:srgbClr val="FFFF8C"/>
+          </a:solidFill>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDot"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1" i="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="131" name="TextBox 130"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19623900" y="2911928"/>
+            <a:ext cx="1403445" cy="286014"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Inner</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Function</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="86" name="TextBox 85"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19623900" y="2490107"/>
+            <a:ext cx="1403445" cy="331856"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>User</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> Input</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="101" name="타원 100"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19206082" y="3415392"/>
+            <a:ext cx="312964" cy="312964"/>
+          </a:xfrm>
+          <a:prstGeom prst="ellipse">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="bg2">
+              <a:lumMod val="90000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="102" name="TextBox 101"/>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19623900" y="3306535"/>
+            <a:ext cx="1403445" cy="530943"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="0" i="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Function Executer</a:t>
+            </a:r>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="0" i="1" u="none">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="139" name="모서리가 둥근 직사각형 138"/>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="19206082" y="2530928"/>
+            <a:ext cx="299358" cy="204107"/>
+          </a:xfrm>
+          <a:prstGeom prst="roundRect">
+            <a:avLst>
+              <a:gd name="adj" fmla="val 0"/>
+            </a:avLst>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent3">
               <a:lumMod val="40000"/>
               <a:lumOff val="60000"/>
             </a:schemeClr>
           </a:solidFill>
-          <a:prstDash val="dash"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:endParaRPr lang="ko-KR" altLang="en-US" sz="2800" b="1" i="1"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
+          <a:ln w="28575">
+            <a:solidFill>
+              <a:schemeClr val="accent4">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="dash"/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent2"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent2"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:endParaRPr lang="ko-KR" altLang="en-US" sz="2800" b="1" i="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -3678,11 +3366,11 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1"/>
-            <a:t>Function 6)</a:t>
+            <a:t>Function 5)</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1400" b="1" i="1" baseline="0"/>
-            <a:t> Finish Business on day</a:t>
+            <a:t> End of business</a:t>
           </a:r>
           <a:endParaRPr lang="ko-KR" altLang="en-US" sz="1400" b="1" i="1"/>
         </a:p>
@@ -3752,13 +3440,8 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
-            <a:t>Finish</a:t>
+            <a:t>End of Business</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1" baseline="0"/>
-            <a:t> Bussiness</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" altLang="ko-KR" sz="1600" b="0" i="1"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -5506,7 +5189,7 @@
   </sheetPr>
   <dimension ref="B1:AV20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -6171,52 +5854,52 @@
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="93" t="str">
         <f>Index!$C$10</f>
         <v>Header</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="71" t="str">
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="91" t="str">
         <f>Index!$AB$10</f>
         <v>Project Image</v>
       </c>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="73" t="s">
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="75">
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="95">
         <f>Index!$AK$18</f>
         <v>43955</v>
       </c>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="73" t="s">
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="71" t="str">
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="91" t="str">
         <f>Index!$AQ$18</f>
         <v>Rick</v>
       </c>
-      <c r="AD2" s="71"/>
-      <c r="AE2" s="71"/>
+      <c r="AD2" s="91"/>
+      <c r="AE2" s="91"/>
       <c r="AF2" s="34"/>
       <c r="AG2" s="34"/>
       <c r="AH2" s="34"/>
@@ -6227,36 +5910,36 @@
       <c r="AM2" s="35"/>
     </row>
     <row r="3" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="72"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="72"/>
-      <c r="L3" s="72"/>
-      <c r="M3" s="72"/>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="74"/>
-      <c r="Q3" s="74"/>
-      <c r="R3" s="74"/>
-      <c r="S3" s="74"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="76"/>
-      <c r="X3" s="76"/>
-      <c r="Y3" s="76"/>
-      <c r="Z3" s="74"/>
-      <c r="AA3" s="74"/>
-      <c r="AB3" s="74"/>
-      <c r="AC3" s="72"/>
-      <c r="AD3" s="72"/>
-      <c r="AE3" s="72"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="94"/>
+      <c r="E3" s="94"/>
+      <c r="F3" s="94"/>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="92"/>
+      <c r="K3" s="92"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
+      <c r="N3" s="92"/>
+      <c r="O3" s="92"/>
+      <c r="P3" s="94"/>
+      <c r="Q3" s="94"/>
+      <c r="R3" s="94"/>
+      <c r="S3" s="94"/>
+      <c r="T3" s="96"/>
+      <c r="U3" s="96"/>
+      <c r="V3" s="96"/>
+      <c r="W3" s="96"/>
+      <c r="X3" s="96"/>
+      <c r="Y3" s="96"/>
+      <c r="Z3" s="94"/>
+      <c r="AA3" s="94"/>
+      <c r="AB3" s="94"/>
+      <c r="AC3" s="92"/>
+      <c r="AD3" s="92"/>
+      <c r="AE3" s="92"/>
       <c r="AJ3" s="36"/>
       <c r="AK3" s="36"/>
       <c r="AL3" s="36"/>
@@ -6295,52 +5978,52 @@
     </row>
     <row r="5" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35"/>
-      <c r="B5" s="82" t="s">
+      <c r="B5" s="81" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="83"/>
-      <c r="D5" s="84" t="s">
+      <c r="C5" s="82"/>
+      <c r="D5" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="85" t="s">
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="85"/>
-      <c r="J5" s="85"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="85"/>
-      <c r="M5" s="85"/>
-      <c r="N5" s="85" t="s">
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
+      <c r="N5" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="O5" s="85"/>
-      <c r="P5" s="85"/>
-      <c r="Q5" s="85"/>
-      <c r="R5" s="85"/>
-      <c r="S5" s="85"/>
-      <c r="T5" s="85"/>
-      <c r="U5" s="85"/>
-      <c r="V5" s="85"/>
-      <c r="W5" s="85"/>
-      <c r="X5" s="85"/>
-      <c r="Y5" s="85"/>
-      <c r="Z5" s="85"/>
-      <c r="AA5" s="85"/>
-      <c r="AB5" s="85" t="s">
+      <c r="O5" s="84"/>
+      <c r="P5" s="84"/>
+      <c r="Q5" s="84"/>
+      <c r="R5" s="84"/>
+      <c r="S5" s="84"/>
+      <c r="T5" s="84"/>
+      <c r="U5" s="84"/>
+      <c r="V5" s="84"/>
+      <c r="W5" s="84"/>
+      <c r="X5" s="84"/>
+      <c r="Y5" s="84"/>
+      <c r="Z5" s="84"/>
+      <c r="AA5" s="84"/>
+      <c r="AB5" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="AC5" s="85"/>
-      <c r="AD5" s="85"/>
-      <c r="AE5" s="85"/>
-      <c r="AF5" s="85" t="s">
+      <c r="AC5" s="84"/>
+      <c r="AD5" s="84"/>
+      <c r="AE5" s="84"/>
+      <c r="AF5" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="AG5" s="85"/>
-      <c r="AH5" s="85"/>
-      <c r="AI5" s="86"/>
+      <c r="AG5" s="84"/>
+      <c r="AH5" s="84"/>
+      <c r="AI5" s="85"/>
       <c r="AJ5" s="37"/>
       <c r="AK5" s="37"/>
       <c r="AL5" s="37"/>
@@ -6359,50 +6042,50 @@
     </row>
     <row r="6" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="35"/>
-      <c r="B6" s="77">
+      <c r="B6" s="86">
         <v>1</v>
       </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="79">
+      <c r="C6" s="87"/>
+      <c r="D6" s="88">
         <v>43955</v>
       </c>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="80" t="s">
+      <c r="E6" s="88"/>
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="80"/>
-      <c r="J6" s="80"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="80"/>
-      <c r="M6" s="80"/>
-      <c r="N6" s="80"/>
-      <c r="O6" s="80"/>
-      <c r="P6" s="80"/>
-      <c r="Q6" s="80"/>
-      <c r="R6" s="80"/>
-      <c r="S6" s="80"/>
-      <c r="T6" s="80"/>
-      <c r="U6" s="80"/>
-      <c r="V6" s="80"/>
-      <c r="W6" s="80"/>
-      <c r="X6" s="80"/>
-      <c r="Y6" s="80"/>
-      <c r="Z6" s="80"/>
-      <c r="AA6" s="80"/>
-      <c r="AB6" s="80" t="s">
+      <c r="I6" s="89"/>
+      <c r="J6" s="89"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="89"/>
+      <c r="M6" s="89"/>
+      <c r="N6" s="89"/>
+      <c r="O6" s="89"/>
+      <c r="P6" s="89"/>
+      <c r="Q6" s="89"/>
+      <c r="R6" s="89"/>
+      <c r="S6" s="89"/>
+      <c r="T6" s="89"/>
+      <c r="U6" s="89"/>
+      <c r="V6" s="89"/>
+      <c r="W6" s="89"/>
+      <c r="X6" s="89"/>
+      <c r="Y6" s="89"/>
+      <c r="Z6" s="89"/>
+      <c r="AA6" s="89"/>
+      <c r="AB6" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="AC6" s="80"/>
-      <c r="AD6" s="80"/>
-      <c r="AE6" s="80"/>
-      <c r="AF6" s="80" t="s">
+      <c r="AC6" s="89"/>
+      <c r="AD6" s="89"/>
+      <c r="AE6" s="89"/>
+      <c r="AF6" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="AG6" s="80"/>
-      <c r="AH6" s="80"/>
-      <c r="AI6" s="81"/>
+      <c r="AG6" s="89"/>
+      <c r="AH6" s="89"/>
+      <c r="AI6" s="90"/>
       <c r="AJ6" s="37"/>
       <c r="AL6" s="36"/>
       <c r="AM6" s="36"/>
@@ -6419,42 +6102,42 @@
     </row>
     <row r="7" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35"/>
-      <c r="B7" s="87">
+      <c r="B7" s="71">
         <v>2</v>
       </c>
-      <c r="C7" s="88"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="89"/>
-      <c r="F7" s="89"/>
-      <c r="G7" s="89"/>
-      <c r="H7" s="90"/>
-      <c r="I7" s="90"/>
-      <c r="J7" s="90"/>
-      <c r="K7" s="90"/>
-      <c r="L7" s="90"/>
-      <c r="M7" s="90"/>
-      <c r="N7" s="90"/>
-      <c r="O7" s="90"/>
-      <c r="P7" s="90"/>
-      <c r="Q7" s="90"/>
-      <c r="R7" s="90"/>
-      <c r="S7" s="90"/>
-      <c r="T7" s="90"/>
-      <c r="U7" s="90"/>
-      <c r="V7" s="90"/>
-      <c r="W7" s="90"/>
-      <c r="X7" s="90"/>
-      <c r="Y7" s="90"/>
-      <c r="Z7" s="90"/>
-      <c r="AA7" s="90"/>
-      <c r="AB7" s="90"/>
-      <c r="AC7" s="90"/>
-      <c r="AD7" s="90"/>
-      <c r="AE7" s="90"/>
-      <c r="AF7" s="90"/>
-      <c r="AG7" s="90"/>
-      <c r="AH7" s="90"/>
-      <c r="AI7" s="91"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
+      <c r="O7" s="74"/>
+      <c r="P7" s="74"/>
+      <c r="Q7" s="74"/>
+      <c r="R7" s="74"/>
+      <c r="S7" s="74"/>
+      <c r="T7" s="74"/>
+      <c r="U7" s="74"/>
+      <c r="V7" s="74"/>
+      <c r="W7" s="74"/>
+      <c r="X7" s="74"/>
+      <c r="Y7" s="74"/>
+      <c r="Z7" s="74"/>
+      <c r="AA7" s="74"/>
+      <c r="AB7" s="74"/>
+      <c r="AC7" s="74"/>
+      <c r="AD7" s="74"/>
+      <c r="AE7" s="74"/>
+      <c r="AF7" s="74"/>
+      <c r="AG7" s="74"/>
+      <c r="AH7" s="74"/>
+      <c r="AI7" s="75"/>
       <c r="AJ7" s="37"/>
       <c r="AK7" s="37"/>
       <c r="AL7" s="37"/>
@@ -6473,42 +6156,42 @@
     </row>
     <row r="8" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35"/>
-      <c r="B8" s="87">
+      <c r="B8" s="71">
         <v>3</v>
       </c>
-      <c r="C8" s="88"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="89"/>
-      <c r="F8" s="89"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="90"/>
-      <c r="I8" s="90"/>
-      <c r="J8" s="90"/>
-      <c r="K8" s="90"/>
-      <c r="L8" s="90"/>
-      <c r="M8" s="90"/>
-      <c r="N8" s="90"/>
-      <c r="O8" s="90"/>
-      <c r="P8" s="90"/>
-      <c r="Q8" s="90"/>
-      <c r="R8" s="90"/>
-      <c r="S8" s="90"/>
-      <c r="T8" s="90"/>
-      <c r="U8" s="90"/>
-      <c r="V8" s="90"/>
-      <c r="W8" s="90"/>
-      <c r="X8" s="90"/>
-      <c r="Y8" s="90"/>
-      <c r="Z8" s="90"/>
-      <c r="AA8" s="90"/>
-      <c r="AB8" s="90"/>
-      <c r="AC8" s="90"/>
-      <c r="AD8" s="90"/>
-      <c r="AE8" s="90"/>
-      <c r="AF8" s="90"/>
-      <c r="AG8" s="90"/>
-      <c r="AH8" s="90"/>
-      <c r="AI8" s="91"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74"/>
+      <c r="T8" s="74"/>
+      <c r="U8" s="74"/>
+      <c r="V8" s="74"/>
+      <c r="W8" s="74"/>
+      <c r="X8" s="74"/>
+      <c r="Y8" s="74"/>
+      <c r="Z8" s="74"/>
+      <c r="AA8" s="74"/>
+      <c r="AB8" s="74"/>
+      <c r="AC8" s="74"/>
+      <c r="AD8" s="74"/>
+      <c r="AE8" s="74"/>
+      <c r="AF8" s="74"/>
+      <c r="AG8" s="74"/>
+      <c r="AH8" s="74"/>
+      <c r="AI8" s="75"/>
       <c r="AJ8" s="37"/>
       <c r="AK8" s="37"/>
       <c r="AL8" s="37"/>
@@ -6527,42 +6210,42 @@
     </row>
     <row r="9" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="35"/>
-      <c r="B9" s="87">
+      <c r="B9" s="71">
         <v>4</v>
       </c>
-      <c r="C9" s="88"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="90"/>
-      <c r="I9" s="90"/>
-      <c r="J9" s="90"/>
-      <c r="K9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
-      <c r="N9" s="90"/>
-      <c r="O9" s="90"/>
-      <c r="P9" s="90"/>
-      <c r="Q9" s="90"/>
-      <c r="R9" s="90"/>
-      <c r="S9" s="90"/>
-      <c r="T9" s="90"/>
-      <c r="U9" s="90"/>
-      <c r="V9" s="90"/>
-      <c r="W9" s="90"/>
-      <c r="X9" s="90"/>
-      <c r="Y9" s="90"/>
-      <c r="Z9" s="90"/>
-      <c r="AA9" s="90"/>
-      <c r="AB9" s="90"/>
-      <c r="AC9" s="90"/>
-      <c r="AD9" s="90"/>
-      <c r="AE9" s="90"/>
-      <c r="AF9" s="90"/>
-      <c r="AG9" s="90"/>
-      <c r="AH9" s="90"/>
-      <c r="AI9" s="91"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73"/>
+      <c r="H9" s="74"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
+      <c r="L9" s="74"/>
+      <c r="M9" s="74"/>
+      <c r="N9" s="74"/>
+      <c r="O9" s="74"/>
+      <c r="P9" s="74"/>
+      <c r="Q9" s="74"/>
+      <c r="R9" s="74"/>
+      <c r="S9" s="74"/>
+      <c r="T9" s="74"/>
+      <c r="U9" s="74"/>
+      <c r="V9" s="74"/>
+      <c r="W9" s="74"/>
+      <c r="X9" s="74"/>
+      <c r="Y9" s="74"/>
+      <c r="Z9" s="74"/>
+      <c r="AA9" s="74"/>
+      <c r="AB9" s="74"/>
+      <c r="AC9" s="74"/>
+      <c r="AD9" s="74"/>
+      <c r="AE9" s="74"/>
+      <c r="AF9" s="74"/>
+      <c r="AG9" s="74"/>
+      <c r="AH9" s="74"/>
+      <c r="AI9" s="75"/>
       <c r="AJ9" s="37"/>
       <c r="AK9" s="37"/>
       <c r="AL9" s="37"/>
@@ -6581,42 +6264,42 @@
     </row>
     <row r="10" spans="1:50" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="35"/>
-      <c r="B10" s="92">
+      <c r="B10" s="76">
         <v>5</v>
       </c>
-      <c r="C10" s="93"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="94"/>
-      <c r="H10" s="95"/>
-      <c r="I10" s="95"/>
-      <c r="J10" s="95"/>
-      <c r="K10" s="95"/>
-      <c r="L10" s="95"/>
-      <c r="M10" s="95"/>
-      <c r="N10" s="95"/>
-      <c r="O10" s="95"/>
-      <c r="P10" s="95"/>
-      <c r="Q10" s="95"/>
-      <c r="R10" s="95"/>
-      <c r="S10" s="95"/>
-      <c r="T10" s="95"/>
-      <c r="U10" s="95"/>
-      <c r="V10" s="95"/>
-      <c r="W10" s="95"/>
-      <c r="X10" s="95"/>
-      <c r="Y10" s="95"/>
-      <c r="Z10" s="95"/>
-      <c r="AA10" s="95"/>
-      <c r="AB10" s="95"/>
-      <c r="AC10" s="95"/>
-      <c r="AD10" s="95"/>
-      <c r="AE10" s="95"/>
-      <c r="AF10" s="95"/>
-      <c r="AG10" s="95"/>
-      <c r="AH10" s="95"/>
-      <c r="AI10" s="96"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="79"/>
+      <c r="I10" s="79"/>
+      <c r="J10" s="79"/>
+      <c r="K10" s="79"/>
+      <c r="L10" s="79"/>
+      <c r="M10" s="79"/>
+      <c r="N10" s="79"/>
+      <c r="O10" s="79"/>
+      <c r="P10" s="79"/>
+      <c r="Q10" s="79"/>
+      <c r="R10" s="79"/>
+      <c r="S10" s="79"/>
+      <c r="T10" s="79"/>
+      <c r="U10" s="79"/>
+      <c r="V10" s="79"/>
+      <c r="W10" s="79"/>
+      <c r="X10" s="79"/>
+      <c r="Y10" s="79"/>
+      <c r="Z10" s="79"/>
+      <c r="AA10" s="79"/>
+      <c r="AB10" s="79"/>
+      <c r="AC10" s="79"/>
+      <c r="AD10" s="79"/>
+      <c r="AE10" s="79"/>
+      <c r="AF10" s="79"/>
+      <c r="AG10" s="79"/>
+      <c r="AH10" s="79"/>
+      <c r="AI10" s="80"/>
       <c r="AJ10" s="38"/>
       <c r="AK10" s="38"/>
       <c r="AL10" s="38"/>
@@ -7027,42 +6710,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:G9"/>
-    <mergeCell ref="H9:AA9"/>
-    <mergeCell ref="AB9:AE9"/>
-    <mergeCell ref="AF9:AI9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="H10:AA10"/>
-    <mergeCell ref="AB10:AE10"/>
-    <mergeCell ref="AF10:AI10"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="H7:AA7"/>
-    <mergeCell ref="AB7:AE7"/>
-    <mergeCell ref="AF7:AI7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:AA8"/>
-    <mergeCell ref="AB8:AE8"/>
-    <mergeCell ref="AF8:AI8"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="H5:AA5"/>
-    <mergeCell ref="AB5:AE5"/>
-    <mergeCell ref="AF5:AI5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="H6:AA6"/>
-    <mergeCell ref="AB6:AE6"/>
-    <mergeCell ref="AF6:AI6"/>
     <mergeCell ref="AC2:AE3"/>
     <mergeCell ref="B2:H3"/>
     <mergeCell ref="I2:O3"/>
     <mergeCell ref="P2:S3"/>
     <mergeCell ref="T2:Y3"/>
     <mergeCell ref="Z2:AB3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:G6"/>
+    <mergeCell ref="H6:AA6"/>
+    <mergeCell ref="AB6:AE6"/>
+    <mergeCell ref="AF6:AI6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="H5:AA5"/>
+    <mergeCell ref="AB5:AE5"/>
+    <mergeCell ref="AF5:AI5"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:G8"/>
+    <mergeCell ref="H8:AA8"/>
+    <mergeCell ref="AB8:AE8"/>
+    <mergeCell ref="AF8:AI8"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:G7"/>
+    <mergeCell ref="H7:AA7"/>
+    <mergeCell ref="AB7:AE7"/>
+    <mergeCell ref="AF7:AI7"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="H10:AA10"/>
+    <mergeCell ref="AB10:AE10"/>
+    <mergeCell ref="AF10:AI10"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:G9"/>
+    <mergeCell ref="H9:AA9"/>
+    <mergeCell ref="AB9:AE9"/>
+    <mergeCell ref="AF9:AI9"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -7082,7 +6765,7 @@
   </sheetPr>
   <dimension ref="B1:CJ46"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7096,52 +6779,52 @@
   <sheetData>
     <row r="1" spans="2:88" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:88" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="93" t="str">
         <f>Index!$C$10</f>
         <v>Header</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="71" t="str">
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="91" t="str">
         <f>Index!$AB$10</f>
         <v>Project Image</v>
       </c>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="73" t="s">
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="75">
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="95">
         <f>Index!$AK$18</f>
         <v>43955</v>
       </c>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="73" t="s">
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="71" t="str">
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="91" t="str">
         <f>Index!$AQ$18</f>
         <v>Rick</v>
       </c>
-      <c r="AD2" s="71"/>
-      <c r="AE2" s="71"/>
+      <c r="AD2" s="91"/>
+      <c r="AE2" s="91"/>
     </row>
     <row r="3" spans="2:88" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="97"/>
@@ -7214,21 +6897,21 @@
       <c r="AE4" s="48"/>
     </row>
     <row r="5" spans="2:88" s="10" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
       <c r="Q5" s="44"/>
       <c r="R5" s="44"/>
       <c r="S5" s="44"/>
@@ -10737,52 +10420,52 @@
   <sheetData>
     <row r="1" spans="2:88" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:88" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="73" t="str">
+      <c r="B2" s="93" t="str">
         <f>Index!$C$10</f>
         <v>Header</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="71" t="str">
+      <c r="C2" s="93"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+      <c r="I2" s="91" t="str">
         <f>Index!$AB$10</f>
         <v>Project Image</v>
       </c>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="71"/>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="73" t="s">
+      <c r="J2" s="91"/>
+      <c r="K2" s="91"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="91"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="75">
+      <c r="Q2" s="93"/>
+      <c r="R2" s="93"/>
+      <c r="S2" s="93"/>
+      <c r="T2" s="95">
         <f>Index!$AK$18</f>
         <v>43955</v>
       </c>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="73" t="s">
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
+      <c r="Z2" s="93" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="73"/>
-      <c r="AB2" s="73"/>
-      <c r="AC2" s="71" t="str">
+      <c r="AA2" s="93"/>
+      <c r="AB2" s="93"/>
+      <c r="AC2" s="91" t="str">
         <f>Index!$AQ$18</f>
         <v>Rick</v>
       </c>
-      <c r="AD2" s="71"/>
-      <c r="AE2" s="71"/>
+      <c r="AD2" s="91"/>
+      <c r="AE2" s="91"/>
     </row>
     <row r="3" spans="2:88" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="97"/>
@@ -10855,21 +10538,21 @@
       <c r="AE4" s="48"/>
     </row>
     <row r="5" spans="2:88" s="10" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="74"/>
-      <c r="C5" s="74"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="74"/>
-      <c r="N5" s="74"/>
-      <c r="O5" s="74"/>
-      <c r="P5" s="74"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
       <c r="Q5" s="44"/>
       <c r="R5" s="44"/>
       <c r="S5" s="44"/>

</xml_diff>